<commit_message>
Modifico archivo sspmi/data.xlsx según cambios del 2017-09-26
</commit_message>
<xml_diff>
--- a/sspmi/data.xlsx
+++ b/sspmi/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="285" windowWidth="14535" windowHeight="7365" tabRatio="748" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="285" windowWidth="14535" windowHeight="7365" tabRatio="748" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="catalog" sheetId="16" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4392" uniqueCount="1022">
   <si>
     <t>distribution_identifier</t>
   </si>
@@ -3210,6 +3210,9 @@
   </si>
   <si>
     <t>población, tasa, mortalidad, natalidad, alumnos, empleo, depósitos, préstamos, gastos, recursos, datos provinciales</t>
+  </si>
+  <si>
+    <t>2017-09-26</t>
   </si>
 </sst>
 </file>
@@ -4749,7 +4752,7 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5220,9 +5223,6 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="4" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="40" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6279,11 +6279,11 @@
   <dimension ref="A1:AA97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:XFD1"/>
       <selection pane="topRight" sqref="A1:XFD1"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9176,8 +9176,8 @@
   </sheetPr>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C14" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" topLeftCell="D14" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10082,10 +10082,10 @@
         <v>32</v>
       </c>
       <c r="L15" s="48" t="s">
-        <v>897</v>
+        <v>1021</v>
       </c>
       <c r="M15" s="48" t="s">
-        <v>897</v>
+        <v>1021</v>
       </c>
       <c r="N15" s="65" t="s">
         <v>33</v>
@@ -10141,11 +10141,11 @@
       <c r="K16" s="169" t="s">
         <v>32</v>
       </c>
-      <c r="L16" s="171" t="s">
-        <v>897</v>
-      </c>
-      <c r="M16" s="171" t="s">
-        <v>897</v>
+      <c r="L16" s="48" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M16" s="48" t="s">
+        <v>1021</v>
       </c>
       <c r="N16" s="169" t="s">
         <v>33</v>
@@ -10153,10 +10153,10 @@
       <c r="O16" s="169" t="s">
         <v>34</v>
       </c>
-      <c r="P16" s="172" t="s">
+      <c r="P16" s="171" t="s">
         <v>965</v>
       </c>
-      <c r="Q16" s="173" t="s">
+      <c r="Q16" s="172" t="s">
         <v>38</v>
       </c>
       <c r="R16" s="49"/>
@@ -10187,12 +10187,12 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="K32" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E14" sqref="E14"/>
       <selection pane="topRight" activeCell="E14" sqref="E14"/>
       <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35:N36"/>
+      <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11462,20 +11462,24 @@
       <c r="E35" s="67" t="s">
         <v>968</v>
       </c>
-      <c r="F35" s="173" t="s">
+      <c r="F35" s="172" t="s">
         <v>898</v>
       </c>
-      <c r="G35" s="174" t="s">
+      <c r="G35" s="173" t="s">
         <v>49</v>
       </c>
-      <c r="H35" s="173" t="s">
+      <c r="H35" s="172" t="s">
         <v>38</v>
       </c>
       <c r="I35" s="56"/>
       <c r="J35" s="49"/>
       <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
+      <c r="L35" s="48" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M35" s="48" t="s">
+        <v>1021</v>
+      </c>
       <c r="N35" s="49"/>
     </row>
     <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.2">
@@ -11494,20 +11498,24 @@
       <c r="E36" s="67" t="s">
         <v>970</v>
       </c>
-      <c r="F36" s="173" t="s">
+      <c r="F36" s="172" t="s">
         <v>898</v>
       </c>
-      <c r="G36" s="174" t="s">
+      <c r="G36" s="173" t="s">
         <v>49</v>
       </c>
-      <c r="H36" s="173" t="s">
+      <c r="H36" s="172" t="s">
         <v>38</v>
       </c>
       <c r="I36" s="56"/>
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
+      <c r="L36" s="48" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M36" s="48" t="s">
+        <v>1021</v>
+      </c>
       <c r="N36" s="49"/>
     </row>
   </sheetData>
@@ -22481,740 +22489,740 @@
       <c r="H423" s="61"/>
     </row>
     <row r="424" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A424" s="180" t="s">
+      <c r="A424" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B424" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C424" s="176" t="s">
+      <c r="C424" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D424" s="178" t="s">
+      <c r="D424" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E424" s="177" t="s">
+      <c r="E424" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="F424" s="175" t="s">
+      <c r="F424" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="G424" s="175" t="s">
+      <c r="G424" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="H424" s="175"/>
+      <c r="H424" s="174"/>
     </row>
     <row r="425" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A425" s="180" t="s">
+      <c r="A425" s="179" t="s">
         <v>963</v>
       </c>
-      <c r="B425" s="175" t="s">
+      <c r="B425" s="174" t="s">
         <v>964</v>
       </c>
-      <c r="C425" s="176" t="s">
+      <c r="C425" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D425" s="177" t="s">
+      <c r="D425" s="176" t="s">
         <v>968</v>
       </c>
-      <c r="E425" s="177" t="s">
+      <c r="E425" s="176" t="s">
         <v>971</v>
       </c>
-      <c r="F425" s="175" t="s">
+      <c r="F425" s="174" t="s">
         <v>972</v>
       </c>
-      <c r="G425" s="175" t="s">
+      <c r="G425" s="174" t="s">
         <v>973</v>
       </c>
-      <c r="H425" s="175"/>
+      <c r="H425" s="174"/>
     </row>
     <row r="426" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A426" s="180" t="s">
+      <c r="A426" s="179" t="s">
         <v>963</v>
       </c>
-      <c r="B426" s="175" t="s">
+      <c r="B426" s="174" t="s">
         <v>964</v>
       </c>
-      <c r="C426" s="176" t="s">
+      <c r="C426" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D426" s="177" t="s">
+      <c r="D426" s="176" t="s">
         <v>968</v>
       </c>
-      <c r="E426" s="177" t="s">
+      <c r="E426" s="176" t="s">
         <v>974</v>
       </c>
-      <c r="F426" s="175" t="s">
+      <c r="F426" s="174" t="s">
         <v>972</v>
       </c>
-      <c r="G426" s="175" t="s">
+      <c r="G426" s="174" t="s">
         <v>975</v>
       </c>
-      <c r="H426" s="175"/>
+      <c r="H426" s="174"/>
     </row>
     <row r="427" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A427" s="180" t="s">
+      <c r="A427" s="179" t="s">
         <v>963</v>
       </c>
-      <c r="B427" s="175" t="s">
+      <c r="B427" s="174" t="s">
         <v>964</v>
       </c>
-      <c r="C427" s="176" t="s">
+      <c r="C427" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D427" s="177" t="s">
+      <c r="D427" s="176" t="s">
         <v>968</v>
       </c>
-      <c r="E427" s="177" t="s">
+      <c r="E427" s="176" t="s">
         <v>976</v>
       </c>
-      <c r="F427" s="175" t="s">
+      <c r="F427" s="174" t="s">
         <v>972</v>
       </c>
-      <c r="G427" s="175" t="s">
+      <c r="G427" s="174" t="s">
         <v>977</v>
       </c>
-      <c r="H427" s="175"/>
+      <c r="H427" s="174"/>
     </row>
     <row r="428" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A428" s="180" t="s">
+      <c r="A428" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B428" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C428" s="176" t="s">
+      <c r="C428" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D428" s="178" t="s">
+      <c r="D428" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E428" s="177" t="s">
+      <c r="E428" s="176" t="s">
         <v>978</v>
       </c>
-      <c r="F428" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G428" s="175" t="s">
+      <c r="F428" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G428" s="174" t="s">
         <v>979</v>
       </c>
-      <c r="H428" s="181" t="s">
+      <c r="H428" s="180" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="429" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A429" s="180" t="s">
+      <c r="A429" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B429" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C429" s="176" t="s">
+      <c r="C429" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D429" s="178" t="s">
+      <c r="D429" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E429" s="177" t="s">
+      <c r="E429" s="176" t="s">
         <v>980</v>
       </c>
-      <c r="F429" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G429" s="175" t="s">
+      <c r="F429" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G429" s="174" t="s">
         <v>981</v>
       </c>
-      <c r="H429" s="181" t="s">
+      <c r="H429" s="180" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="430" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A430" s="180" t="s">
+      <c r="A430" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B430" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C430" s="176" t="s">
+      <c r="C430" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D430" s="178" t="s">
+      <c r="D430" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E430" s="177" t="s">
+      <c r="E430" s="176" t="s">
         <v>982</v>
       </c>
-      <c r="F430" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G430" s="175" t="s">
+      <c r="F430" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G430" s="174" t="s">
         <v>983</v>
       </c>
-      <c r="H430" s="181" t="s">
+      <c r="H430" s="180" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="431" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A431" s="180" t="s">
+      <c r="A431" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B431" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C431" s="176" t="s">
+      <c r="C431" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D431" s="178" t="s">
+      <c r="D431" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E431" s="177" t="s">
+      <c r="E431" s="176" t="s">
         <v>984</v>
       </c>
-      <c r="F431" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G431" s="175" t="s">
+      <c r="F431" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G431" s="174" t="s">
         <v>985</v>
       </c>
-      <c r="H431" s="175" t="s">
+      <c r="H431" s="174" t="s">
         <v>944</v>
       </c>
     </row>
     <row r="432" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A432" s="180" t="s">
+      <c r="A432" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B432" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C432" s="176" t="s">
+      <c r="C432" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D432" s="178" t="s">
+      <c r="D432" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E432" s="177" t="s">
+      <c r="E432" s="176" t="s">
         <v>986</v>
       </c>
-      <c r="F432" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G432" s="175" t="s">
+      <c r="F432" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G432" s="174" t="s">
         <v>987</v>
       </c>
-      <c r="H432" s="181" t="s">
+      <c r="H432" s="180" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="433" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A433" s="180" t="s">
+      <c r="A433" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B433" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C433" s="176" t="s">
+      <c r="C433" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D433" s="178" t="s">
+      <c r="D433" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E433" s="177" t="s">
+      <c r="E433" s="176" t="s">
         <v>988</v>
       </c>
-      <c r="F433" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G433" s="175" t="s">
+      <c r="F433" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G433" s="174" t="s">
         <v>989</v>
       </c>
-      <c r="H433" s="181" t="s">
+      <c r="H433" s="180" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="434" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A434" s="180" t="s">
+      <c r="A434" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B434" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C434" s="176" t="s">
+      <c r="C434" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D434" s="178" t="s">
+      <c r="D434" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E434" s="177" t="s">
+      <c r="E434" s="176" t="s">
         <v>990</v>
       </c>
-      <c r="F434" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G434" s="175" t="s">
+      <c r="F434" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G434" s="174" t="s">
         <v>991</v>
       </c>
-      <c r="H434" s="181" t="s">
+      <c r="H434" s="180" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="435" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A435" s="180" t="s">
+      <c r="A435" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B435" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C435" s="176" t="s">
+      <c r="C435" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D435" s="178" t="s">
+      <c r="D435" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E435" s="177" t="s">
+      <c r="E435" s="176" t="s">
         <v>992</v>
       </c>
-      <c r="F435" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G435" s="175" t="s">
+      <c r="F435" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G435" s="174" t="s">
         <v>993</v>
       </c>
-      <c r="H435" s="181" t="s">
+      <c r="H435" s="180" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="436" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A436" s="180" t="s">
+      <c r="A436" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B436" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C436" s="176" t="s">
+      <c r="C436" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D436" s="178" t="s">
+      <c r="D436" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E436" s="177" t="s">
+      <c r="E436" s="176" t="s">
         <v>994</v>
       </c>
-      <c r="F436" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G436" s="175" t="s">
+      <c r="F436" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G436" s="174" t="s">
         <v>995</v>
       </c>
-      <c r="H436" s="175" t="s">
+      <c r="H436" s="174" t="s">
         <v>946</v>
       </c>
     </row>
     <row r="437" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A437" s="180" t="s">
+      <c r="A437" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B437" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C437" s="176" t="s">
+      <c r="C437" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D437" s="178" t="s">
+      <c r="D437" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E437" s="177" t="s">
+      <c r="E437" s="176" t="s">
         <v>996</v>
       </c>
-      <c r="F437" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G437" s="175" t="s">
+      <c r="F437" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G437" s="174" t="s">
         <v>997</v>
       </c>
-      <c r="H437" s="175" t="s">
+      <c r="H437" s="174" t="s">
         <v>946</v>
       </c>
     </row>
     <row r="438" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A438" s="180" t="s">
+      <c r="A438" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B438" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C438" s="176" t="s">
+      <c r="C438" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D438" s="178" t="s">
+      <c r="D438" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E438" s="177" t="s">
+      <c r="E438" s="176" t="s">
         <v>998</v>
       </c>
-      <c r="F438" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G438" s="175" t="s">
+      <c r="F438" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G438" s="174" t="s">
         <v>999</v>
       </c>
-      <c r="H438" s="175" t="s">
+      <c r="H438" s="174" t="s">
         <v>946</v>
       </c>
     </row>
     <row r="439" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A439" s="180" t="s">
+      <c r="A439" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B439" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C439" s="176" t="s">
+      <c r="C439" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D439" s="178" t="s">
+      <c r="D439" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E439" s="177" t="s">
+      <c r="E439" s="176" t="s">
         <v>1000</v>
       </c>
-      <c r="F439" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G439" s="175" t="s">
+      <c r="F439" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G439" s="174" t="s">
         <v>1001</v>
       </c>
-      <c r="H439" s="182" t="s">
+      <c r="H439" s="181" t="s">
         <v>866</v>
       </c>
     </row>
     <row r="440" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A440" s="180" t="s">
+      <c r="A440" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B440" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C440" s="176" t="s">
+      <c r="C440" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D440" s="178" t="s">
+      <c r="D440" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E440" s="177" t="s">
+      <c r="E440" s="176" t="s">
         <v>1002</v>
       </c>
-      <c r="F440" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G440" s="175" t="s">
+      <c r="F440" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G440" s="174" t="s">
         <v>1003</v>
       </c>
-      <c r="H440" s="179" t="s">
+      <c r="H440" s="178" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="441" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A441" s="180" t="s">
+      <c r="A441" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B441" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C441" s="176" t="s">
+      <c r="C441" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D441" s="178" t="s">
+      <c r="D441" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E441" s="177" t="s">
+      <c r="E441" s="176" t="s">
         <v>1004</v>
       </c>
-      <c r="F441" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G441" s="175" t="s">
+      <c r="F441" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G441" s="174" t="s">
         <v>1005</v>
       </c>
-      <c r="H441" s="179" t="s">
+      <c r="H441" s="178" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="442" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A442" s="180" t="s">
+      <c r="A442" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B442" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C442" s="176" t="s">
+      <c r="C442" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D442" s="178" t="s">
+      <c r="D442" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E442" s="177" t="s">
+      <c r="E442" s="176" t="s">
         <v>1006</v>
       </c>
-      <c r="F442" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G442" s="175" t="s">
+      <c r="F442" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G442" s="174" t="s">
         <v>1007</v>
       </c>
-      <c r="H442" s="179" t="s">
+      <c r="H442" s="178" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="443" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A443" s="180" t="s">
+      <c r="A443" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B443" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C443" s="176" t="s">
+      <c r="C443" s="175" t="s">
         <v>967</v>
       </c>
-      <c r="D443" s="178" t="s">
+      <c r="D443" s="177" t="s">
         <v>968</v>
       </c>
-      <c r="E443" s="177" t="s">
+      <c r="E443" s="176" t="s">
         <v>1008</v>
       </c>
-      <c r="F443" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G443" s="175" t="s">
+      <c r="F443" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G443" s="174" t="s">
         <v>1009</v>
       </c>
-      <c r="H443" s="179" t="s">
+      <c r="H443" s="178" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="444" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A444" s="180" t="s">
+      <c r="A444" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B444" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C444" s="176" t="s">
+      <c r="C444" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D444" s="178" t="s">
+      <c r="D444" s="177" t="s">
         <v>970</v>
       </c>
-      <c r="E444" s="177" t="s">
+      <c r="E444" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="F444" s="175" t="s">
+      <c r="F444" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="G444" s="175" t="s">
+      <c r="G444" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="H444" s="175"/>
+      <c r="H444" s="174"/>
     </row>
     <row r="445" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A445" s="180" t="s">
+      <c r="A445" s="179" t="s">
         <v>963</v>
       </c>
-      <c r="B445" s="175" t="s">
+      <c r="B445" s="174" t="s">
         <v>964</v>
       </c>
-      <c r="C445" s="176" t="s">
+      <c r="C445" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D445" s="177" t="s">
+      <c r="D445" s="176" t="s">
         <v>970</v>
       </c>
-      <c r="E445" s="177" t="s">
+      <c r="E445" s="176" t="s">
         <v>971</v>
       </c>
-      <c r="F445" s="175" t="s">
+      <c r="F445" s="174" t="s">
         <v>972</v>
       </c>
-      <c r="G445" s="175" t="s">
+      <c r="G445" s="174" t="s">
         <v>973</v>
       </c>
-      <c r="H445" s="175"/>
+      <c r="H445" s="174"/>
     </row>
     <row r="446" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A446" s="180" t="s">
+      <c r="A446" s="179" t="s">
         <v>963</v>
       </c>
-      <c r="B446" s="175" t="s">
+      <c r="B446" s="174" t="s">
         <v>964</v>
       </c>
-      <c r="C446" s="176" t="s">
+      <c r="C446" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D446" s="177" t="s">
+      <c r="D446" s="176" t="s">
         <v>970</v>
       </c>
-      <c r="E446" s="177" t="s">
+      <c r="E446" s="176" t="s">
         <v>974</v>
       </c>
-      <c r="F446" s="175" t="s">
+      <c r="F446" s="174" t="s">
         <v>972</v>
       </c>
-      <c r="G446" s="175" t="s">
+      <c r="G446" s="174" t="s">
         <v>975</v>
       </c>
-      <c r="H446" s="175"/>
+      <c r="H446" s="174"/>
     </row>
     <row r="447" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A447" s="180" t="s">
+      <c r="A447" s="179" t="s">
         <v>963</v>
       </c>
-      <c r="B447" s="175" t="s">
+      <c r="B447" s="174" t="s">
         <v>964</v>
       </c>
-      <c r="C447" s="176" t="s">
+      <c r="C447" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D447" s="177" t="s">
+      <c r="D447" s="176" t="s">
         <v>970</v>
       </c>
-      <c r="E447" s="177" t="s">
+      <c r="E447" s="176" t="s">
         <v>976</v>
       </c>
-      <c r="F447" s="175" t="s">
+      <c r="F447" s="174" t="s">
         <v>972</v>
       </c>
-      <c r="G447" s="175" t="s">
+      <c r="G447" s="174" t="s">
         <v>977</v>
       </c>
-      <c r="H447" s="175"/>
+      <c r="H447" s="174"/>
     </row>
     <row r="448" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A448" s="180" t="s">
+      <c r="A448" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B448" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C448" s="176" t="s">
+      <c r="C448" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D448" s="178" t="s">
+      <c r="D448" s="177" t="s">
         <v>970</v>
       </c>
-      <c r="E448" s="177" t="s">
+      <c r="E448" s="176" t="s">
         <v>1000</v>
       </c>
-      <c r="F448" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G448" s="175" t="s">
+      <c r="F448" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G448" s="174" t="s">
         <v>1010</v>
       </c>
-      <c r="H448" s="182" t="s">
+      <c r="H448" s="181" t="s">
         <v>866</v>
       </c>
     </row>
     <row r="449" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A449" s="180" t="s">
+      <c r="A449" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B449" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C449" s="176" t="s">
+      <c r="C449" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D449" s="178" t="s">
+      <c r="D449" s="177" t="s">
         <v>970</v>
       </c>
-      <c r="E449" s="177" t="s">
+      <c r="E449" s="176" t="s">
         <v>1011</v>
       </c>
-      <c r="F449" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G449" s="175" t="s">
+      <c r="F449" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G449" s="174" t="s">
         <v>1012</v>
       </c>
-      <c r="H449" s="181" t="s">
+      <c r="H449" s="180" t="s">
         <v>947</v>
       </c>
     </row>
     <row r="450" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A450" s="180" t="s">
+      <c r="A450" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B450" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C450" s="176" t="s">
+      <c r="C450" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D450" s="178" t="s">
+      <c r="D450" s="177" t="s">
         <v>970</v>
       </c>
-      <c r="E450" s="177" t="s">
+      <c r="E450" s="176" t="s">
         <v>1013</v>
       </c>
-      <c r="F450" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G450" s="175" t="s">
+      <c r="F450" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G450" s="174" t="s">
         <v>1014</v>
       </c>
-      <c r="H450" s="181" t="s">
+      <c r="H450" s="180" t="s">
         <v>947</v>
       </c>
     </row>
     <row r="451" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A451" s="180" t="s">
+      <c r="A451" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B451" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C451" s="176" t="s">
+      <c r="C451" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D451" s="178" t="s">
+      <c r="D451" s="177" t="s">
         <v>970</v>
       </c>
-      <c r="E451" s="177" t="s">
+      <c r="E451" s="176" t="s">
         <v>1015</v>
       </c>
-      <c r="F451" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G451" s="175" t="s">
+      <c r="F451" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G451" s="174" t="s">
         <v>1016</v>
       </c>
-      <c r="H451" s="181" t="s">
+      <c r="H451" s="180" t="s">
         <v>947</v>
       </c>
     </row>
     <row r="452" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A452" s="180" t="s">
+      <c r="A452" s="179" t="s">
         <v>963</v>
       </c>
       <c r="B452" s="103" t="s">
         <v>964</v>
       </c>
-      <c r="C452" s="176" t="s">
+      <c r="C452" s="175" t="s">
         <v>969</v>
       </c>
-      <c r="D452" s="178" t="s">
+      <c r="D452" s="177" t="s">
         <v>970</v>
       </c>
-      <c r="E452" s="177" t="s">
+      <c r="E452" s="176" t="s">
         <v>1017</v>
       </c>
-      <c r="F452" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G452" s="175" t="s">
+      <c r="F452" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G452" s="174" t="s">
         <v>1018</v>
       </c>
-      <c r="H452" s="181" t="s">
+      <c r="H452" s="180" t="s">
         <v>947</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modifico archivo sspmi/data.xlsx según cambios del 2017-09-27
</commit_message>
<xml_diff>
--- a/sspmi/data.xlsx
+++ b/sspmi/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="285" windowWidth="14535" windowHeight="7365" tabRatio="748" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="285" windowWidth="14535" windowHeight="7365" tabRatio="748" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="catalog" sheetId="16" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4392" uniqueCount="1022">
   <si>
     <t>distribution_identifier</t>
   </si>
@@ -2843,9 +2843,6 @@
     <t>2017-09-25</t>
   </si>
   <si>
-    <t>https://minhacienda.gob.ar/datos/</t>
-  </si>
-  <si>
     <t>Indicadores forestales, muebles y papel en valores trimestrales</t>
   </si>
   <si>
@@ -3210,6 +3207,12 @@
   </si>
   <si>
     <t>población, tasa, mortalidad, natalidad, alumnos, empleo, depósitos, préstamos, gastos, recursos, datos provinciales</t>
+  </si>
+  <si>
+    <t>2017-09-26</t>
+  </si>
+  <si>
+    <t>https://www.minhacienda.gob.ar/secretarias/politica-economica/programacion-microeconomica/datos-microeconomicos/</t>
   </si>
 </sst>
 </file>
@@ -4749,7 +4752,7 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5220,9 +5223,6 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="4" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="40" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6279,11 +6279,11 @@
   <dimension ref="A1:AA97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:XFD1"/>
       <selection pane="topRight" sqref="A1:XFD1"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9176,8 +9176,8 @@
   </sheetPr>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C14" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" topLeftCell="O1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -9296,7 +9296,7 @@
         <v>71</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="K2" s="35" t="s">
         <v>32</v>
@@ -9356,7 +9356,7 @@
         <v>85</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="K3" s="35" t="s">
         <v>32</v>
@@ -9416,7 +9416,7 @@
         <v>114</v>
       </c>
       <c r="J4" s="53" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="K4" s="65" t="s">
         <v>32</v>
@@ -9476,7 +9476,7 @@
         <v>169</v>
       </c>
       <c r="J5" s="53" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="K5" s="65" t="s">
         <v>32</v>
@@ -9536,7 +9536,7 @@
         <v>169</v>
       </c>
       <c r="J6" s="53" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K6" s="65" t="s">
         <v>32</v>
@@ -9596,7 +9596,7 @@
         <v>340</v>
       </c>
       <c r="J7" s="53" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="K7" s="65" t="s">
         <v>32</v>
@@ -9656,7 +9656,7 @@
         <v>443</v>
       </c>
       <c r="J8" s="53" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="K8" s="65" t="s">
         <v>32</v>
@@ -9716,7 +9716,7 @@
         <v>476</v>
       </c>
       <c r="J9" s="53" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="K9" s="65" t="s">
         <v>32</v>
@@ -9776,7 +9776,7 @@
         <v>340</v>
       </c>
       <c r="J10" s="53" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="K10" s="65" t="s">
         <v>32</v>
@@ -9836,7 +9836,7 @@
         <v>340</v>
       </c>
       <c r="J11" s="53" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="K11" s="65" t="s">
         <v>32</v>
@@ -9896,7 +9896,7 @@
         <v>641</v>
       </c>
       <c r="J12" s="53" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="K12" s="65" t="s">
         <v>32</v>
@@ -9956,7 +9956,7 @@
         <v>169</v>
       </c>
       <c r="J13" s="53" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="K13" s="85" t="s">
         <v>32</v>
@@ -10016,7 +10016,7 @@
         <v>114</v>
       </c>
       <c r="J14" s="53" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="K14" s="65" t="s">
         <v>32</v>
@@ -10076,16 +10076,16 @@
         <v>85</v>
       </c>
       <c r="J15" s="53" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="K15" s="65" t="s">
         <v>32</v>
       </c>
       <c r="L15" s="48" t="s">
-        <v>897</v>
+        <v>1020</v>
       </c>
       <c r="M15" s="48" t="s">
-        <v>897</v>
+        <v>1020</v>
       </c>
       <c r="N15" s="65" t="s">
         <v>33</v>
@@ -10109,13 +10109,13 @@
     </row>
     <row r="16" spans="1:20" ht="90" x14ac:dyDescent="0.2">
       <c r="A16" s="167" t="s">
+        <v>962</v>
+      </c>
+      <c r="B16" s="59" t="s">
         <v>963</v>
       </c>
-      <c r="B16" s="59" t="s">
-        <v>964</v>
-      </c>
       <c r="C16" s="59" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D16" s="168" t="s">
         <v>36</v>
@@ -10133,19 +10133,19 @@
         <v>31</v>
       </c>
       <c r="I16" s="170" t="s">
+        <v>1018</v>
+      </c>
+      <c r="J16" s="67" t="s">
         <v>1019</v>
-      </c>
-      <c r="J16" s="67" t="s">
-        <v>1020</v>
       </c>
       <c r="K16" s="169" t="s">
         <v>32</v>
       </c>
-      <c r="L16" s="171" t="s">
-        <v>897</v>
-      </c>
-      <c r="M16" s="171" t="s">
-        <v>897</v>
+      <c r="L16" s="48" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M16" s="48" t="s">
+        <v>1020</v>
       </c>
       <c r="N16" s="169" t="s">
         <v>33</v>
@@ -10153,15 +10153,15 @@
       <c r="O16" s="169" t="s">
         <v>34</v>
       </c>
-      <c r="P16" s="172" t="s">
-        <v>965</v>
-      </c>
-      <c r="Q16" s="173" t="s">
+      <c r="P16" s="171" t="s">
+        <v>964</v>
+      </c>
+      <c r="Q16" s="172" t="s">
         <v>38</v>
       </c>
       <c r="R16" s="49"/>
       <c r="S16" s="67" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="T16" s="169" t="s">
         <v>35</v>
@@ -10187,12 +10187,12 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E14" sqref="E14"/>
       <selection pane="topRight" activeCell="E14" sqref="E14"/>
       <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35:N36"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10275,7 +10275,7 @@
         <v>56</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G2" s="37" t="s">
         <v>49</v>
@@ -10294,7 +10294,7 @@
       </c>
       <c r="N2" s="14"/>
     </row>
-    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>51</v>
       </c>
@@ -10311,7 +10311,7 @@
         <v>57</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>49</v>
@@ -10330,7 +10330,7 @@
       </c>
       <c r="N3" s="14"/>
     </row>
-    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>51</v>
       </c>
@@ -10347,7 +10347,7 @@
         <v>63</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>49</v>
@@ -10366,7 +10366,7 @@
       </c>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A5" s="50" t="s">
         <v>82</v>
       </c>
@@ -10383,7 +10383,7 @@
         <v>89</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G5" s="54" t="s">
         <v>49</v>
@@ -10402,7 +10402,7 @@
       </c>
       <c r="N5" s="49"/>
     </row>
-    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="50" t="s">
         <v>82</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>91</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G6" s="54" t="s">
         <v>49</v>
@@ -10438,7 +10438,7 @@
       </c>
       <c r="N6" s="49"/>
     </row>
-    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A7" s="50" t="s">
         <v>112</v>
       </c>
@@ -10455,7 +10455,7 @@
         <v>118</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G7" s="54" t="s">
         <v>49</v>
@@ -10474,7 +10474,7 @@
       </c>
       <c r="N7" s="49"/>
     </row>
-    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A8" s="50" t="s">
         <v>112</v>
       </c>
@@ -10491,7 +10491,7 @@
         <v>120</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G8" s="54" t="s">
         <v>49</v>
@@ -10510,7 +10510,7 @@
       </c>
       <c r="N8" s="49"/>
     </row>
-    <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A9" s="50" t="s">
         <v>112</v>
       </c>
@@ -10527,7 +10527,7 @@
         <v>122</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G9" s="54" t="s">
         <v>49</v>
@@ -10546,7 +10546,7 @@
       </c>
       <c r="N9" s="49"/>
     </row>
-    <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A10" s="50" t="s">
         <v>167</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>173</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G10" s="54" t="s">
         <v>49</v>
@@ -10582,7 +10582,7 @@
       </c>
       <c r="N10" s="49"/>
     </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A11" s="50" t="s">
         <v>167</v>
       </c>
@@ -10599,7 +10599,7 @@
         <v>175</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G11" s="54" t="s">
         <v>49</v>
@@ -10618,7 +10618,7 @@
       </c>
       <c r="N11" s="49"/>
     </row>
-    <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A12" s="50" t="s">
         <v>167</v>
       </c>
@@ -10635,7 +10635,7 @@
         <v>177</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G12" s="54" t="s">
         <v>49</v>
@@ -10654,7 +10654,7 @@
       </c>
       <c r="N12" s="49"/>
     </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A13" s="50" t="s">
         <v>215</v>
       </c>
@@ -10671,7 +10671,7 @@
         <v>220</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G13" s="54" t="s">
         <v>49</v>
@@ -10690,7 +10690,7 @@
       </c>
       <c r="N13" s="49"/>
     </row>
-    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A14" s="50" t="s">
         <v>215</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>222</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G14" s="54" t="s">
         <v>49</v>
@@ -10726,7 +10726,7 @@
       </c>
       <c r="N14" s="49"/>
     </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A15" s="50" t="s">
         <v>215</v>
       </c>
@@ -10743,7 +10743,7 @@
         <v>225</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G15" s="54" t="s">
         <v>49</v>
@@ -10762,7 +10762,7 @@
       </c>
       <c r="N15" s="49"/>
     </row>
-    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A16" s="50" t="s">
         <v>338</v>
       </c>
@@ -10779,7 +10779,7 @@
         <v>344</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G16" s="54" t="s">
         <v>49</v>
@@ -10798,7 +10798,7 @@
       </c>
       <c r="N16" s="49"/>
     </row>
-    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A17" s="50" t="s">
         <v>338</v>
       </c>
@@ -10815,7 +10815,7 @@
         <v>346</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G17" s="54" t="s">
         <v>49</v>
@@ -10834,7 +10834,7 @@
       </c>
       <c r="N17" s="49"/>
     </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A18" s="50" t="s">
         <v>441</v>
       </c>
@@ -10851,7 +10851,7 @@
         <v>447</v>
       </c>
       <c r="F18" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G18" s="54" t="s">
         <v>49</v>
@@ -10870,7 +10870,7 @@
       </c>
       <c r="N18" s="49"/>
     </row>
-    <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
         <v>95</v>
       </c>
@@ -10887,7 +10887,7 @@
         <v>480</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G19" s="54" t="s">
         <v>49</v>
@@ -10906,7 +10906,7 @@
       </c>
       <c r="N19" s="49"/>
     </row>
-    <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A20" s="50" t="s">
         <v>95</v>
       </c>
@@ -10923,7 +10923,7 @@
         <v>482</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G20" s="54" t="s">
         <v>49</v>
@@ -10942,7 +10942,7 @@
       </c>
       <c r="N20" s="49"/>
     </row>
-    <row r="21" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A21" s="50" t="s">
         <v>72</v>
       </c>
@@ -10959,7 +10959,7 @@
         <v>506</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G21" s="54" t="s">
         <v>49</v>
@@ -10978,7 +10978,7 @@
       </c>
       <c r="N21" s="49"/>
     </row>
-    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A22" s="50" t="s">
         <v>72</v>
       </c>
@@ -10989,13 +10989,13 @@
         <v>507</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E22" s="53" t="s">
         <v>508</v>
       </c>
       <c r="F22" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G22" s="54" t="s">
         <v>49</v>
@@ -11014,7 +11014,7 @@
       </c>
       <c r="N22" s="49"/>
     </row>
-    <row r="23" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A23" s="50" t="s">
         <v>618</v>
       </c>
@@ -11031,7 +11031,7 @@
         <v>623</v>
       </c>
       <c r="F23" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G23" s="54" t="s">
         <v>49</v>
@@ -11050,7 +11050,7 @@
       </c>
       <c r="N23" s="49"/>
     </row>
-    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A24" s="50" t="s">
         <v>618</v>
       </c>
@@ -11067,7 +11067,7 @@
         <v>626</v>
       </c>
       <c r="F24" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G24" s="54" t="s">
         <v>49</v>
@@ -11086,7 +11086,7 @@
       </c>
       <c r="N24" s="49"/>
     </row>
-    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A25" s="50" t="s">
         <v>639</v>
       </c>
@@ -11103,7 +11103,7 @@
         <v>645</v>
       </c>
       <c r="F25" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G25" s="54" t="s">
         <v>49</v>
@@ -11122,7 +11122,7 @@
       </c>
       <c r="N25" s="49"/>
     </row>
-    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A26" s="50" t="s">
         <v>639</v>
       </c>
@@ -11139,7 +11139,7 @@
         <v>647</v>
       </c>
       <c r="F26" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G26" s="54" t="s">
         <v>49</v>
@@ -11158,7 +11158,7 @@
       </c>
       <c r="N26" s="49"/>
     </row>
-    <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A27" s="50" t="s">
         <v>639</v>
       </c>
@@ -11175,7 +11175,7 @@
         <v>649</v>
       </c>
       <c r="F27" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G27" s="54" t="s">
         <v>49</v>
@@ -11194,7 +11194,7 @@
       </c>
       <c r="N27" s="49"/>
     </row>
-    <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A28" s="50" t="s">
         <v>661</v>
       </c>
@@ -11211,7 +11211,7 @@
         <v>666</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G28" s="54" t="s">
         <v>49</v>
@@ -11230,7 +11230,7 @@
       </c>
       <c r="N28" s="49"/>
     </row>
-    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A29" s="50" t="s">
         <v>661</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>668</v>
       </c>
       <c r="F29" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G29" s="54" t="s">
         <v>49</v>
@@ -11266,7 +11266,7 @@
       </c>
       <c r="N29" s="49"/>
     </row>
-    <row r="30" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A30" s="50" t="s">
         <v>737</v>
       </c>
@@ -11283,7 +11283,7 @@
         <v>741</v>
       </c>
       <c r="F30" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G30" s="54" t="s">
         <v>49</v>
@@ -11302,7 +11302,7 @@
       </c>
       <c r="N30" s="49"/>
     </row>
-    <row r="31" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A31" s="50" t="s">
         <v>737</v>
       </c>
@@ -11319,7 +11319,7 @@
         <v>743</v>
       </c>
       <c r="F31" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G31" s="54" t="s">
         <v>49</v>
@@ -11338,7 +11338,7 @@
       </c>
       <c r="N31" s="86"/>
     </row>
-    <row r="32" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A32" s="50" t="s">
         <v>766</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>771</v>
       </c>
       <c r="F32" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G32" s="54" t="s">
         <v>49</v>
@@ -11374,7 +11374,7 @@
       </c>
       <c r="N32" s="49"/>
     </row>
-    <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A33" s="50" t="s">
         <v>766</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>773</v>
       </c>
       <c r="F33" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G33" s="54" t="s">
         <v>49</v>
@@ -11410,7 +11410,7 @@
       </c>
       <c r="N33" s="49"/>
     </row>
-    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A34" s="50" t="s">
         <v>766</v>
       </c>
@@ -11427,7 +11427,7 @@
         <v>775</v>
       </c>
       <c r="F34" s="36" t="s">
-        <v>898</v>
+        <v>1021</v>
       </c>
       <c r="G34" s="54" t="s">
         <v>49</v>
@@ -11446,76 +11446,81 @@
       </c>
       <c r="N34" s="49"/>
     </row>
-    <row r="35" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A35" s="167" t="s">
+        <v>962</v>
+      </c>
+      <c r="B35" s="59" t="s">
         <v>963</v>
       </c>
-      <c r="B35" s="59" t="s">
-        <v>964</v>
-      </c>
       <c r="C35" s="169" t="s">
+        <v>966</v>
+      </c>
+      <c r="D35" s="67" t="s">
         <v>967</v>
       </c>
-      <c r="D35" s="67" t="s">
-        <v>968</v>
-      </c>
       <c r="E35" s="67" t="s">
-        <v>968</v>
-      </c>
-      <c r="F35" s="173" t="s">
-        <v>898</v>
-      </c>
-      <c r="G35" s="174" t="s">
+        <v>967</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G35" s="173" t="s">
         <v>49</v>
       </c>
-      <c r="H35" s="173" t="s">
+      <c r="H35" s="172" t="s">
         <v>38</v>
       </c>
       <c r="I35" s="56"/>
       <c r="J35" s="49"/>
       <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
+      <c r="L35" s="48" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M35" s="48" t="s">
+        <v>1020</v>
+      </c>
       <c r="N35" s="49"/>
     </row>
-    <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A36" s="167" t="s">
+        <v>962</v>
+      </c>
+      <c r="B36" s="59" t="s">
         <v>963</v>
       </c>
-      <c r="B36" s="59" t="s">
-        <v>964</v>
-      </c>
       <c r="C36" s="169" t="s">
+        <v>968</v>
+      </c>
+      <c r="D36" s="67" t="s">
         <v>969</v>
       </c>
-      <c r="D36" s="67" t="s">
-        <v>970</v>
-      </c>
       <c r="E36" s="67" t="s">
-        <v>970</v>
-      </c>
-      <c r="F36" s="173" t="s">
-        <v>898</v>
-      </c>
-      <c r="G36" s="174" t="s">
+        <v>969</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G36" s="173" t="s">
         <v>49</v>
       </c>
-      <c r="H36" s="173" t="s">
+      <c r="H36" s="172" t="s">
         <v>38</v>
       </c>
       <c r="I36" s="56"/>
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
+      <c r="L36" s="48" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M36" s="48" t="s">
+        <v>1020</v>
+      </c>
       <c r="N36" s="49"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3:F34" r:id="rId2" display="https://minhacienda.gob.ar/datos/"/>
-    <hyperlink ref="F35" r:id="rId3"/>
-    <hyperlink ref="F36" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294"/>
@@ -19501,7 +19506,7 @@
         <v>507</v>
       </c>
       <c r="D308" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E308" s="67" t="s">
         <v>557</v>
@@ -19527,7 +19532,7 @@
         <v>507</v>
       </c>
       <c r="D309" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E309" s="67" t="s">
         <v>559</v>
@@ -19553,7 +19558,7 @@
         <v>507</v>
       </c>
       <c r="D310" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E310" s="67" t="s">
         <v>561</v>
@@ -19579,7 +19584,7 @@
         <v>507</v>
       </c>
       <c r="D311" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E311" s="67" t="s">
         <v>563</v>
@@ -19605,7 +19610,7 @@
         <v>507</v>
       </c>
       <c r="D312" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E312" s="67" t="s">
         <v>565</v>
@@ -19631,7 +19636,7 @@
         <v>507</v>
       </c>
       <c r="D313" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E313" s="67" t="s">
         <v>567</v>
@@ -19657,7 +19662,7 @@
         <v>507</v>
       </c>
       <c r="D314" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E314" s="67" t="s">
         <v>569</v>
@@ -19683,7 +19688,7 @@
         <v>507</v>
       </c>
       <c r="D315" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E315" s="67" t="s">
         <v>571</v>
@@ -19709,7 +19714,7 @@
         <v>507</v>
       </c>
       <c r="D316" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E316" s="67" t="s">
         <v>573</v>
@@ -19735,7 +19740,7 @@
         <v>507</v>
       </c>
       <c r="D317" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E317" s="67" t="s">
         <v>575</v>
@@ -19761,7 +19766,7 @@
         <v>507</v>
       </c>
       <c r="D318" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E318" s="67" t="s">
         <v>577</v>
@@ -19787,7 +19792,7 @@
         <v>507</v>
       </c>
       <c r="D319" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E319" s="67" t="s">
         <v>579</v>
@@ -19813,7 +19818,7 @@
         <v>507</v>
       </c>
       <c r="D320" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E320" s="67" t="s">
         <v>1</v>
@@ -22481,741 +22486,741 @@
       <c r="H423" s="61"/>
     </row>
     <row r="424" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A424" s="180" t="s">
+      <c r="A424" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B424" s="103" t="s">
         <v>963</v>
       </c>
-      <c r="B424" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C424" s="176" t="s">
+      <c r="C424" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D424" s="177" t="s">
         <v>967</v>
       </c>
-      <c r="D424" s="178" t="s">
+      <c r="E424" s="176" t="s">
+        <v>1</v>
+      </c>
+      <c r="F424" s="174" t="s">
+        <v>9</v>
+      </c>
+      <c r="G424" s="174" t="s">
+        <v>10</v>
+      </c>
+      <c r="H424" s="174"/>
+    </row>
+    <row r="425" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A425" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B425" s="174" t="s">
+        <v>963</v>
+      </c>
+      <c r="C425" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D425" s="176" t="s">
+        <v>967</v>
+      </c>
+      <c r="E425" s="176" t="s">
+        <v>970</v>
+      </c>
+      <c r="F425" s="174" t="s">
+        <v>971</v>
+      </c>
+      <c r="G425" s="174" t="s">
+        <v>972</v>
+      </c>
+      <c r="H425" s="174"/>
+    </row>
+    <row r="426" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A426" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B426" s="174" t="s">
+        <v>963</v>
+      </c>
+      <c r="C426" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D426" s="176" t="s">
+        <v>967</v>
+      </c>
+      <c r="E426" s="176" t="s">
+        <v>973</v>
+      </c>
+      <c r="F426" s="174" t="s">
+        <v>971</v>
+      </c>
+      <c r="G426" s="174" t="s">
+        <v>974</v>
+      </c>
+      <c r="H426" s="174"/>
+    </row>
+    <row r="427" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A427" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B427" s="174" t="s">
+        <v>963</v>
+      </c>
+      <c r="C427" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D427" s="176" t="s">
+        <v>967</v>
+      </c>
+      <c r="E427" s="176" t="s">
+        <v>975</v>
+      </c>
+      <c r="F427" s="174" t="s">
+        <v>971</v>
+      </c>
+      <c r="G427" s="174" t="s">
+        <v>976</v>
+      </c>
+      <c r="H427" s="174"/>
+    </row>
+    <row r="428" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A428" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B428" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C428" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D428" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E428" s="176" t="s">
+        <v>977</v>
+      </c>
+      <c r="F428" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G428" s="174" t="s">
+        <v>978</v>
+      </c>
+      <c r="H428" s="180" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="429" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A429" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B429" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C429" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D429" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E429" s="176" t="s">
+        <v>979</v>
+      </c>
+      <c r="F429" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G429" s="174" t="s">
+        <v>980</v>
+      </c>
+      <c r="H429" s="180" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="430" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A430" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B430" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C430" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D430" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E430" s="176" t="s">
+        <v>981</v>
+      </c>
+      <c r="F430" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G430" s="174" t="s">
+        <v>982</v>
+      </c>
+      <c r="H430" s="180" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="431" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A431" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B431" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C431" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D431" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E431" s="176" t="s">
+        <v>983</v>
+      </c>
+      <c r="F431" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G431" s="174" t="s">
+        <v>984</v>
+      </c>
+      <c r="H431" s="174" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="432" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A432" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B432" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C432" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D432" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E432" s="176" t="s">
+        <v>985</v>
+      </c>
+      <c r="F432" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G432" s="174" t="s">
+        <v>986</v>
+      </c>
+      <c r="H432" s="180" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="433" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A433" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B433" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C433" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D433" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E433" s="176" t="s">
+        <v>987</v>
+      </c>
+      <c r="F433" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G433" s="174" t="s">
+        <v>988</v>
+      </c>
+      <c r="H433" s="180" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="434" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A434" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B434" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C434" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D434" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E434" s="176" t="s">
+        <v>989</v>
+      </c>
+      <c r="F434" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G434" s="174" t="s">
+        <v>990</v>
+      </c>
+      <c r="H434" s="180" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="435" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A435" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B435" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C435" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D435" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E435" s="176" t="s">
+        <v>991</v>
+      </c>
+      <c r="F435" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G435" s="174" t="s">
+        <v>992</v>
+      </c>
+      <c r="H435" s="180" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="436" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A436" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B436" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C436" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D436" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E436" s="176" t="s">
+        <v>993</v>
+      </c>
+      <c r="F436" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G436" s="174" t="s">
+        <v>994</v>
+      </c>
+      <c r="H436" s="174" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="437" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A437" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B437" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C437" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D437" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E437" s="176" t="s">
+        <v>995</v>
+      </c>
+      <c r="F437" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G437" s="174" t="s">
+        <v>996</v>
+      </c>
+      <c r="H437" s="174" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="438" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A438" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B438" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C438" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D438" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E438" s="176" t="s">
+        <v>997</v>
+      </c>
+      <c r="F438" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G438" s="174" t="s">
+        <v>998</v>
+      </c>
+      <c r="H438" s="174" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="439" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A439" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B439" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C439" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D439" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E439" s="176" t="s">
+        <v>999</v>
+      </c>
+      <c r="F439" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G439" s="174" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H439" s="181" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="440" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A440" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B440" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C440" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D440" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E440" s="176" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F440" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G440" s="174" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H440" s="178" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="441" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A441" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B441" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C441" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D441" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E441" s="176" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F441" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G441" s="174" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H441" s="178" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="442" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A442" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B442" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C442" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D442" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E442" s="176" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F442" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G442" s="174" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H442" s="178" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="443" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A443" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B443" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C443" s="175" t="s">
+        <v>966</v>
+      </c>
+      <c r="D443" s="177" t="s">
+        <v>967</v>
+      </c>
+      <c r="E443" s="176" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F443" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G443" s="174" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H443" s="178" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="444" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A444" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B444" s="103" t="s">
+        <v>963</v>
+      </c>
+      <c r="C444" s="175" t="s">
         <v>968</v>
       </c>
-      <c r="E424" s="177" t="s">
+      <c r="D444" s="177" t="s">
+        <v>969</v>
+      </c>
+      <c r="E444" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="F424" s="175" t="s">
+      <c r="F444" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="G424" s="175" t="s">
-        <v>10</v>
-      </c>
-      <c r="H424" s="175"/>
-    </row>
-    <row r="425" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A425" s="180" t="s">
+      <c r="G444" s="174" t="s">
+        <v>12</v>
+      </c>
+      <c r="H444" s="174"/>
+    </row>
+    <row r="445" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A445" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B445" s="174" t="s">
         <v>963</v>
       </c>
-      <c r="B425" s="175" t="s">
-        <v>964</v>
-      </c>
-      <c r="C425" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D425" s="177" t="s">
+      <c r="C445" s="175" t="s">
         <v>968</v>
       </c>
-      <c r="E425" s="177" t="s">
+      <c r="D445" s="176" t="s">
+        <v>969</v>
+      </c>
+      <c r="E445" s="176" t="s">
+        <v>970</v>
+      </c>
+      <c r="F445" s="174" t="s">
         <v>971</v>
       </c>
-      <c r="F425" s="175" t="s">
+      <c r="G445" s="174" t="s">
         <v>972</v>
       </c>
-      <c r="G425" s="175" t="s">
+      <c r="H445" s="174"/>
+    </row>
+    <row r="446" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A446" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B446" s="174" t="s">
+        <v>963</v>
+      </c>
+      <c r="C446" s="175" t="s">
+        <v>968</v>
+      </c>
+      <c r="D446" s="176" t="s">
+        <v>969</v>
+      </c>
+      <c r="E446" s="176" t="s">
         <v>973</v>
       </c>
-      <c r="H425" s="175"/>
-    </row>
-    <row r="426" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A426" s="180" t="s">
+      <c r="F446" s="174" t="s">
+        <v>971</v>
+      </c>
+      <c r="G446" s="174" t="s">
+        <v>974</v>
+      </c>
+      <c r="H446" s="174"/>
+    </row>
+    <row r="447" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A447" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B447" s="174" t="s">
         <v>963</v>
       </c>
-      <c r="B426" s="175" t="s">
-        <v>964</v>
-      </c>
-      <c r="C426" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D426" s="177" t="s">
+      <c r="C447" s="175" t="s">
         <v>968</v>
       </c>
-      <c r="E426" s="177" t="s">
-        <v>974</v>
-      </c>
-      <c r="F426" s="175" t="s">
-        <v>972</v>
-      </c>
-      <c r="G426" s="175" t="s">
+      <c r="D447" s="176" t="s">
+        <v>969</v>
+      </c>
+      <c r="E447" s="176" t="s">
         <v>975</v>
       </c>
-      <c r="H426" s="175"/>
-    </row>
-    <row r="427" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A427" s="180" t="s">
+      <c r="F447" s="174" t="s">
+        <v>971</v>
+      </c>
+      <c r="G447" s="174" t="s">
+        <v>976</v>
+      </c>
+      <c r="H447" s="174"/>
+    </row>
+    <row r="448" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A448" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B448" s="103" t="s">
         <v>963</v>
       </c>
-      <c r="B427" s="175" t="s">
-        <v>964</v>
-      </c>
-      <c r="C427" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D427" s="177" t="s">
+      <c r="C448" s="175" t="s">
         <v>968</v>
       </c>
-      <c r="E427" s="177" t="s">
-        <v>976</v>
-      </c>
-      <c r="F427" s="175" t="s">
-        <v>972</v>
-      </c>
-      <c r="G427" s="175" t="s">
-        <v>977</v>
-      </c>
-      <c r="H427" s="175"/>
-    </row>
-    <row r="428" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A428" s="180" t="s">
+      <c r="D448" s="177" t="s">
+        <v>969</v>
+      </c>
+      <c r="E448" s="176" t="s">
+        <v>999</v>
+      </c>
+      <c r="F448" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G448" s="174" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H448" s="181" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="449" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A449" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B449" s="103" t="s">
         <v>963</v>
       </c>
-      <c r="B428" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C428" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D428" s="178" t="s">
+      <c r="C449" s="175" t="s">
         <v>968</v>
       </c>
-      <c r="E428" s="177" t="s">
-        <v>978</v>
-      </c>
-      <c r="F428" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G428" s="175" t="s">
-        <v>979</v>
-      </c>
-      <c r="H428" s="181" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="429" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A429" s="180" t="s">
+      <c r="D449" s="177" t="s">
+        <v>969</v>
+      </c>
+      <c r="E449" s="176" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F449" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G449" s="174" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H449" s="180" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="450" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A450" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B450" s="103" t="s">
         <v>963</v>
       </c>
-      <c r="B429" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C429" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D429" s="178" t="s">
+      <c r="C450" s="175" t="s">
         <v>968</v>
       </c>
-      <c r="E429" s="177" t="s">
-        <v>980</v>
-      </c>
-      <c r="F429" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G429" s="175" t="s">
-        <v>981</v>
-      </c>
-      <c r="H429" s="181" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="430" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A430" s="180" t="s">
+      <c r="D450" s="177" t="s">
+        <v>969</v>
+      </c>
+      <c r="E450" s="176" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F450" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G450" s="174" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H450" s="180" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="451" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A451" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B451" s="103" t="s">
         <v>963</v>
       </c>
-      <c r="B430" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C430" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D430" s="178" t="s">
+      <c r="C451" s="175" t="s">
         <v>968</v>
       </c>
-      <c r="E430" s="177" t="s">
-        <v>982</v>
-      </c>
-      <c r="F430" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G430" s="175" t="s">
-        <v>983</v>
-      </c>
-      <c r="H430" s="181" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="431" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A431" s="180" t="s">
+      <c r="D451" s="177" t="s">
+        <v>969</v>
+      </c>
+      <c r="E451" s="176" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F451" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G451" s="174" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H451" s="180" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="452" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A452" s="179" t="s">
+        <v>962</v>
+      </c>
+      <c r="B452" s="103" t="s">
         <v>963</v>
       </c>
-      <c r="B431" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C431" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D431" s="178" t="s">
+      <c r="C452" s="175" t="s">
         <v>968</v>
       </c>
-      <c r="E431" s="177" t="s">
-        <v>984</v>
-      </c>
-      <c r="F431" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G431" s="175" t="s">
-        <v>985</v>
-      </c>
-      <c r="H431" s="175" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="432" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A432" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B432" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C432" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D432" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E432" s="177" t="s">
-        <v>986</v>
-      </c>
-      <c r="F432" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G432" s="175" t="s">
-        <v>987</v>
-      </c>
-      <c r="H432" s="181" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="433" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A433" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B433" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C433" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D433" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E433" s="177" t="s">
-        <v>988</v>
-      </c>
-      <c r="F433" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G433" s="175" t="s">
-        <v>989</v>
-      </c>
-      <c r="H433" s="181" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="434" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A434" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B434" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C434" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D434" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E434" s="177" t="s">
-        <v>990</v>
-      </c>
-      <c r="F434" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G434" s="175" t="s">
-        <v>991</v>
-      </c>
-      <c r="H434" s="181" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="435" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A435" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B435" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C435" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D435" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E435" s="177" t="s">
-        <v>992</v>
-      </c>
-      <c r="F435" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G435" s="175" t="s">
-        <v>993</v>
-      </c>
-      <c r="H435" s="181" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="436" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A436" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B436" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C436" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D436" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E436" s="177" t="s">
-        <v>994</v>
-      </c>
-      <c r="F436" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G436" s="175" t="s">
-        <v>995</v>
-      </c>
-      <c r="H436" s="175" t="s">
+      <c r="D452" s="177" t="s">
+        <v>969</v>
+      </c>
+      <c r="E452" s="176" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F452" s="174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G452" s="174" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H452" s="180" t="s">
         <v>946</v>
-      </c>
-    </row>
-    <row r="437" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A437" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B437" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C437" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D437" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E437" s="177" t="s">
-        <v>996</v>
-      </c>
-      <c r="F437" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G437" s="175" t="s">
-        <v>997</v>
-      </c>
-      <c r="H437" s="175" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="438" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A438" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B438" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C438" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D438" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E438" s="177" t="s">
-        <v>998</v>
-      </c>
-      <c r="F438" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G438" s="175" t="s">
-        <v>999</v>
-      </c>
-      <c r="H438" s="175" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="439" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A439" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B439" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C439" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D439" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E439" s="177" t="s">
-        <v>1000</v>
-      </c>
-      <c r="F439" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G439" s="175" t="s">
-        <v>1001</v>
-      </c>
-      <c r="H439" s="182" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="440" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A440" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B440" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C440" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D440" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E440" s="177" t="s">
-        <v>1002</v>
-      </c>
-      <c r="F440" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G440" s="175" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H440" s="179" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="441" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A441" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B441" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C441" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D441" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E441" s="177" t="s">
-        <v>1004</v>
-      </c>
-      <c r="F441" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G441" s="175" t="s">
-        <v>1005</v>
-      </c>
-      <c r="H441" s="179" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="442" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A442" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B442" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C442" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D442" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E442" s="177" t="s">
-        <v>1006</v>
-      </c>
-      <c r="F442" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G442" s="175" t="s">
-        <v>1007</v>
-      </c>
-      <c r="H442" s="179" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="443" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A443" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B443" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C443" s="176" t="s">
-        <v>967</v>
-      </c>
-      <c r="D443" s="178" t="s">
-        <v>968</v>
-      </c>
-      <c r="E443" s="177" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F443" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G443" s="175" t="s">
-        <v>1009</v>
-      </c>
-      <c r="H443" s="179" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="444" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A444" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B444" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C444" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D444" s="178" t="s">
-        <v>970</v>
-      </c>
-      <c r="E444" s="177" t="s">
-        <v>1</v>
-      </c>
-      <c r="F444" s="175" t="s">
-        <v>9</v>
-      </c>
-      <c r="G444" s="175" t="s">
-        <v>12</v>
-      </c>
-      <c r="H444" s="175"/>
-    </row>
-    <row r="445" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A445" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B445" s="175" t="s">
-        <v>964</v>
-      </c>
-      <c r="C445" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D445" s="177" t="s">
-        <v>970</v>
-      </c>
-      <c r="E445" s="177" t="s">
-        <v>971</v>
-      </c>
-      <c r="F445" s="175" t="s">
-        <v>972</v>
-      </c>
-      <c r="G445" s="175" t="s">
-        <v>973</v>
-      </c>
-      <c r="H445" s="175"/>
-    </row>
-    <row r="446" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A446" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B446" s="175" t="s">
-        <v>964</v>
-      </c>
-      <c r="C446" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D446" s="177" t="s">
-        <v>970</v>
-      </c>
-      <c r="E446" s="177" t="s">
-        <v>974</v>
-      </c>
-      <c r="F446" s="175" t="s">
-        <v>972</v>
-      </c>
-      <c r="G446" s="175" t="s">
-        <v>975</v>
-      </c>
-      <c r="H446" s="175"/>
-    </row>
-    <row r="447" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A447" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B447" s="175" t="s">
-        <v>964</v>
-      </c>
-      <c r="C447" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D447" s="177" t="s">
-        <v>970</v>
-      </c>
-      <c r="E447" s="177" t="s">
-        <v>976</v>
-      </c>
-      <c r="F447" s="175" t="s">
-        <v>972</v>
-      </c>
-      <c r="G447" s="175" t="s">
-        <v>977</v>
-      </c>
-      <c r="H447" s="175"/>
-    </row>
-    <row r="448" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A448" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B448" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C448" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D448" s="178" t="s">
-        <v>970</v>
-      </c>
-      <c r="E448" s="177" t="s">
-        <v>1000</v>
-      </c>
-      <c r="F448" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G448" s="175" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H448" s="182" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="449" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A449" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B449" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C449" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D449" s="178" t="s">
-        <v>970</v>
-      </c>
-      <c r="E449" s="177" t="s">
-        <v>1011</v>
-      </c>
-      <c r="F449" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G449" s="175" t="s">
-        <v>1012</v>
-      </c>
-      <c r="H449" s="181" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="450" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A450" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B450" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C450" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D450" s="178" t="s">
-        <v>970</v>
-      </c>
-      <c r="E450" s="177" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F450" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G450" s="175" t="s">
-        <v>1014</v>
-      </c>
-      <c r="H450" s="181" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="451" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A451" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B451" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C451" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D451" s="178" t="s">
-        <v>970</v>
-      </c>
-      <c r="E451" s="177" t="s">
-        <v>1015</v>
-      </c>
-      <c r="F451" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G451" s="175" t="s">
-        <v>1016</v>
-      </c>
-      <c r="H451" s="181" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="452" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A452" s="180" t="s">
-        <v>963</v>
-      </c>
-      <c r="B452" s="103" t="s">
-        <v>964</v>
-      </c>
-      <c r="C452" s="176" t="s">
-        <v>969</v>
-      </c>
-      <c r="D452" s="178" t="s">
-        <v>970</v>
-      </c>
-      <c r="E452" s="177" t="s">
-        <v>1017</v>
-      </c>
-      <c r="F452" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="G452" s="175" t="s">
-        <v>1018</v>
-      </c>
-      <c r="H452" s="181" t="s">
-        <v>947</v>
       </c>
     </row>
   </sheetData>
@@ -23404,22 +23409,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="104" t="s">
+        <v>899</v>
+      </c>
+      <c r="B1" s="105" t="s">
         <v>900</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="C1" s="106" t="s">
         <v>901</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="D1" s="106" t="s">
         <v>902</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="E1" s="106" t="s">
         <v>903</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="F1" s="106" t="s">
         <v>904</v>
-      </c>
-      <c r="F1" s="106" t="s">
-        <v>905</v>
       </c>
       <c r="G1" s="107"/>
     </row>
@@ -23428,19 +23433,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="110" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C2" s="111">
         <v>1993</v>
       </c>
       <c r="D2" s="111" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E2" s="112">
         <v>1000000</v>
       </c>
       <c r="F2" s="111" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23454,13 +23459,13 @@
         <v>2004</v>
       </c>
       <c r="D3" s="111" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E3" s="112">
         <v>1000000</v>
       </c>
       <c r="F3" s="111" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23472,13 +23477,13 @@
       </c>
       <c r="C4" s="113"/>
       <c r="D4" s="111" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E4" s="112">
         <v>1000000</v>
       </c>
       <c r="F4" s="111" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23486,7 +23491,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="114" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C5" s="113"/>
       <c r="D5" s="111"/>
@@ -23528,7 +23533,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="114" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C8" s="118"/>
       <c r="D8" s="119"/>
@@ -23556,7 +23561,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="114" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C10" s="115"/>
       <c r="D10" s="116"/>
@@ -23584,7 +23589,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="114" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C12" s="115"/>
       <c r="D12" s="116"/>
@@ -23612,7 +23617,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="114" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C14" s="118"/>
       <c r="D14" s="119"/>
@@ -23626,7 +23631,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="114" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C15" s="115"/>
       <c r="D15" s="116"/>
@@ -23640,7 +23645,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="114" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C16" s="115"/>
       <c r="D16" s="116"/>
@@ -23682,7 +23687,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="114" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C19" s="115"/>
       <c r="D19" s="116"/>
@@ -23722,7 +23727,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="114" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C22" s="115"/>
       <c r="D22" s="116"/>
@@ -23736,17 +23741,17 @@
         <v>22</v>
       </c>
       <c r="B23" s="114" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C23" s="115"/>
       <c r="D23" s="111" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E23" s="112">
         <v>1000000</v>
       </c>
       <c r="F23" s="111" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -23754,7 +23759,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="121" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C24" s="115"/>
       <c r="D24" s="116"/>
@@ -23770,7 +23775,7 @@
       </c>
       <c r="C25" s="118"/>
       <c r="D25" s="111" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E25" s="117">
         <v>1</v>
@@ -23788,7 +23793,7 @@
       </c>
       <c r="C26" s="118"/>
       <c r="D26" s="111" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E26" s="112">
         <v>1000000</v>
@@ -23802,7 +23807,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="114" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C27" s="115"/>
       <c r="D27" s="116"/>
@@ -23828,7 +23833,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="125" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C29" s="126"/>
       <c r="D29" s="127"/>
@@ -23860,7 +23865,7 @@
       </c>
       <c r="C31" s="136"/>
       <c r="D31" s="137" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E31" s="138"/>
       <c r="F31" s="139"/>
@@ -23870,7 +23875,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="138" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C32" s="140"/>
       <c r="D32" s="141"/>
@@ -23882,7 +23887,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="138" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C33" s="136"/>
       <c r="D33" s="142"/>
@@ -23894,7 +23899,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="138" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C34" s="136"/>
       <c r="D34" s="143"/>
@@ -23906,7 +23911,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="138" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C35" s="140"/>
       <c r="D35" s="141"/>
@@ -23918,7 +23923,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="138" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C36" s="136"/>
       <c r="D36" s="141"/>
@@ -23930,7 +23935,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="135" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C37" s="136"/>
       <c r="D37" s="141"/>
@@ -23942,7 +23947,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="145" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C38" s="146"/>
       <c r="D38" s="146"/>
@@ -23954,7 +23959,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="149" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C39" s="150"/>
       <c r="D39" s="150"/>
@@ -23966,7 +23971,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="152" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C40" s="153"/>
       <c r="D40" s="154"/>
@@ -23978,7 +23983,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="152" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C41" s="153"/>
       <c r="D41" s="154"/>
@@ -23990,7 +23995,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="152" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C42" s="153"/>
       <c r="D42" s="154"/>
@@ -24002,7 +24007,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="152" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C43" s="153"/>
       <c r="D43" s="154"/>
@@ -24014,7 +24019,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="155" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C44" s="153"/>
       <c r="D44" s="154"/>
@@ -24026,7 +24031,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="155" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C45" s="153"/>
       <c r="D45" s="154"/>
@@ -24038,7 +24043,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="155" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C46" s="153"/>
       <c r="D46" s="154"/>
@@ -24050,7 +24055,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="155" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C47" s="153"/>
       <c r="D47" s="154"/>
@@ -24062,7 +24067,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="155" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C48" s="153"/>
       <c r="D48" s="154"/>
@@ -24074,7 +24079,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="155" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C49" s="153"/>
       <c r="D49" s="154"/>
@@ -24086,7 +24091,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="155" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C50" s="153"/>
       <c r="D50" s="154"/>
@@ -24098,7 +24103,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="155" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C51" s="153"/>
       <c r="D51" s="154"/>
@@ -24110,7 +24115,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="155" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C52" s="153"/>
       <c r="D52" s="154"/>
@@ -24122,7 +24127,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="157" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C53" s="158"/>
       <c r="D53" s="159"/>
@@ -24172,7 +24177,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="163" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C57" s="163"/>
       <c r="D57" s="163"/>
@@ -24194,7 +24199,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="165" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24338,7 +24343,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="165" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24376,7 +24381,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="166" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C72" s="163"/>
       <c r="D72" s="163"/>
@@ -24390,7 +24395,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="166" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C73" s="163"/>
       <c r="D73" s="163"/>
@@ -24404,7 +24409,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="166" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C74" s="163"/>
       <c r="D74" s="163"/>
@@ -24418,7 +24423,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="166" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C75" s="163"/>
       <c r="D75" s="163"/>
@@ -24430,7 +24435,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="166" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C76" s="163"/>
       <c r="D76" s="163"/>
@@ -24444,7 +24449,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="166" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C77" s="163"/>
       <c r="D77" s="163"/>
@@ -24452,7 +24457,7 @@
         <v>1000</v>
       </c>
       <c r="F77" s="165" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24460,7 +24465,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="166" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C78" s="166"/>
       <c r="D78" s="166"/>
@@ -24468,7 +24473,7 @@
         <v>1000</v>
       </c>
       <c r="F78" s="165" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifico archivo sspmi/data.xlsx según cambios del 2017-12-22
</commit_message>
<xml_diff>
--- a/sspmi/data.xlsx
+++ b/sspmi/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="14535" windowHeight="7305" tabRatio="748" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="14535" windowHeight="7305" tabRatio="748" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="catalog" sheetId="16" r:id="rId1"/>
@@ -2945,9 +2945,6 @@
     <t>https://www.minhacienda.gob.ar/catalogo-sspmi/dataset/22-indicadores-lacteo-basecompleta.csv</t>
   </si>
   <si>
-    <t>https://www.minhacienda.gob.ar/catalogo-sspmi/dataset/23-indicadores-manzana-pera-basecompelta.csv</t>
-  </si>
-  <si>
     <t>https://www.minhacienda.gob.ar/catalogo-sspmi/dataset/26-indicadores-metalicas-basicas-basecompleta.csv</t>
   </si>
   <si>
@@ -3888,6 +3885,9 @@
   </si>
   <si>
     <t>corrientes</t>
+  </si>
+  <si>
+    <t>https://www.minhacienda.gob.ar/catalogo-sspmi/dataset/23-indicadores-manzana-pera-basecompleta.csv</t>
   </si>
 </sst>
 </file>
@@ -11018,7 +11018,7 @@
         <v>417</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D3" s="115" t="s">
         <v>34</v>
@@ -11138,7 +11138,7 @@
         <v>418</v>
       </c>
       <c r="C5" s="118" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D5" s="75" t="s">
         <v>34</v>
@@ -11237,7 +11237,7 @@
         <v>32</v>
       </c>
       <c r="P6" s="76" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="Q6" s="78" t="s">
         <v>36</v>
@@ -11738,7 +11738,7 @@
         <v>424</v>
       </c>
       <c r="C15" s="118" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D15" s="75" t="s">
         <v>34</v>
@@ -11798,7 +11798,7 @@
         <v>425</v>
       </c>
       <c r="C16" s="118" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D16" s="75" t="s">
         <v>34</v>
@@ -11915,10 +11915,10 @@
         <v>312</v>
       </c>
       <c r="B18" s="118" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C18" s="118" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D18" s="75" t="s">
         <v>34</v>
@@ -12092,13 +12092,13 @@
     </row>
     <row r="21" spans="1:20" ht="90" x14ac:dyDescent="0.2">
       <c r="A21" s="74" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B21" s="118" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C21" s="118" t="s">
         <v>1020</v>
-      </c>
-      <c r="B21" s="118" t="s">
-        <v>1086</v>
-      </c>
-      <c r="C21" s="118" t="s">
-        <v>1021</v>
       </c>
       <c r="D21" s="75" t="s">
         <v>34</v>
@@ -12119,7 +12119,7 @@
         <v>104</v>
       </c>
       <c r="J21" s="90" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="K21" s="76" t="s">
         <v>30</v>
@@ -12133,14 +12133,14 @@
         <v>32</v>
       </c>
       <c r="P21" s="76" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="Q21" s="78" t="s">
         <v>36</v>
       </c>
       <c r="R21" s="119"/>
       <c r="S21" s="125" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="T21" s="76" t="s">
         <v>33</v>
@@ -12148,13 +12148,13 @@
     </row>
     <row r="22" spans="1:20" ht="90" x14ac:dyDescent="0.2">
       <c r="A22" s="74" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B22" s="118" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C22" s="118" t="s">
         <v>1036</v>
-      </c>
-      <c r="B22" s="118" t="s">
-        <v>1087</v>
-      </c>
-      <c r="C22" s="118" t="s">
-        <v>1037</v>
       </c>
       <c r="D22" s="75" t="s">
         <v>34</v>
@@ -12175,7 +12175,7 @@
         <v>104</v>
       </c>
       <c r="J22" s="90" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="K22" s="76" t="s">
         <v>30</v>
@@ -12189,14 +12189,14 @@
         <v>32</v>
       </c>
       <c r="P22" s="76" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="Q22" s="78" t="s">
         <v>36</v>
       </c>
       <c r="R22" s="119"/>
       <c r="S22" s="125" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="T22" s="76" t="s">
         <v>33</v>
@@ -12204,13 +12204,13 @@
     </row>
     <row r="23" spans="1:20" ht="90" x14ac:dyDescent="0.2">
       <c r="A23" s="74" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B23" s="118" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C23" s="118" t="s">
         <v>1088</v>
-      </c>
-      <c r="C23" s="118" t="s">
-        <v>1089</v>
       </c>
       <c r="D23" s="75" t="s">
         <v>34</v>
@@ -12231,7 +12231,7 @@
         <v>863</v>
       </c>
       <c r="J23" s="90" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="K23" s="76" t="s">
         <v>30</v>
@@ -12245,14 +12245,14 @@
         <v>32</v>
       </c>
       <c r="P23" s="76" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="Q23" s="78" t="s">
         <v>36</v>
       </c>
       <c r="R23" s="119"/>
       <c r="S23" s="125" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="T23" s="76" t="s">
         <v>33</v>
@@ -12260,13 +12260,13 @@
     </row>
     <row r="24" spans="1:20" ht="90" x14ac:dyDescent="0.2">
       <c r="A24" s="74" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B24" s="118" t="s">
         <v>1103</v>
       </c>
-      <c r="B24" s="118" t="s">
-        <v>1104</v>
-      </c>
       <c r="C24" s="118" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D24" s="75" t="s">
         <v>34</v>
@@ -12287,7 +12287,7 @@
         <v>104</v>
       </c>
       <c r="J24" s="90" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="K24" s="76" t="s">
         <v>30</v>
@@ -12301,14 +12301,14 @@
         <v>32</v>
       </c>
       <c r="P24" s="76" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="Q24" s="78" t="s">
         <v>36</v>
       </c>
       <c r="R24" s="119"/>
       <c r="S24" s="125" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="T24" s="76" t="s">
         <v>33</v>
@@ -12316,13 +12316,13 @@
     </row>
     <row r="25" spans="1:20" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="74" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B25" s="118" t="s">
         <v>1179</v>
       </c>
-      <c r="B25" s="118" t="s">
+      <c r="C25" s="118" t="s">
         <v>1180</v>
-      </c>
-      <c r="C25" s="118" t="s">
-        <v>1181</v>
       </c>
       <c r="D25" s="75" t="s">
         <v>34</v>
@@ -12343,7 +12343,7 @@
         <v>104</v>
       </c>
       <c r="J25" s="90" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="K25" s="76" t="s">
         <v>30</v>
@@ -12357,14 +12357,14 @@
         <v>32</v>
       </c>
       <c r="P25" s="76" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="Q25" s="78" t="s">
         <v>36</v>
       </c>
       <c r="R25" s="119"/>
       <c r="S25" s="125" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="T25" s="76" t="s">
         <v>33</v>
@@ -12372,13 +12372,13 @@
     </row>
     <row r="26" spans="1:20" ht="90" x14ac:dyDescent="0.2">
       <c r="A26" s="74" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B26" s="118" t="s">
         <v>1216</v>
       </c>
-      <c r="B26" s="118" t="s">
+      <c r="C26" s="118" t="s">
         <v>1217</v>
-      </c>
-      <c r="C26" s="118" t="s">
-        <v>1218</v>
       </c>
       <c r="D26" s="75" t="s">
         <v>34</v>
@@ -12396,10 +12396,10 @@
         <v>29</v>
       </c>
       <c r="I26" s="77" t="s">
+        <v>1221</v>
+      </c>
+      <c r="J26" s="90" t="s">
         <v>1222</v>
-      </c>
-      <c r="J26" s="90" t="s">
-        <v>1223</v>
       </c>
       <c r="K26" s="76" t="s">
         <v>30</v>
@@ -12413,7 +12413,7 @@
         <v>32</v>
       </c>
       <c r="P26" s="76" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="Q26" s="78" t="s">
         <v>36</v>
@@ -12456,12 +12456,12 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E14" sqref="E14"/>
       <selection pane="topRight" activeCell="E14" sqref="E14"/>
       <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12767,7 +12767,7 @@
         <v>868</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G8" s="79" t="s">
         <v>47</v>
@@ -12915,7 +12915,7 @@
         <v>783</v>
       </c>
       <c r="F12" s="87" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="G12" s="79" t="s">
         <v>47</v>
@@ -12952,7 +12952,7 @@
         <v>855</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="G13" s="79" t="s">
         <v>47</v>
@@ -12989,7 +12989,7 @@
         <v>782</v>
       </c>
       <c r="F14" s="87" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G14" s="79" t="s">
         <v>47</v>
@@ -13100,7 +13100,7 @@
         <v>636</v>
       </c>
       <c r="F17" s="87" t="s">
-        <v>970</v>
+        <v>1284</v>
       </c>
       <c r="G17" s="79" t="s">
         <v>47</v>
@@ -13137,7 +13137,7 @@
         <v>637</v>
       </c>
       <c r="F18" s="87" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="G18" s="79" t="s">
         <v>47</v>
@@ -13174,7 +13174,7 @@
         <v>542</v>
       </c>
       <c r="F19" s="87" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="G19" s="79" t="s">
         <v>47</v>
@@ -13211,7 +13211,7 @@
         <v>638</v>
       </c>
       <c r="F20" s="87" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="G20" s="79" t="s">
         <v>47</v>
@@ -13232,23 +13232,23 @@
     </row>
     <row r="21" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A21" s="74" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B21" s="138" t="str">
         <f>+VLOOKUP(A21,dataset!A21:B38,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C21" s="80" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D21" s="125" t="s">
         <v>1024</v>
       </c>
-      <c r="D21" s="125" t="s">
-        <v>1025</v>
-      </c>
       <c r="E21" s="125" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F21" s="87" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="G21" s="79" t="s">
         <v>47</v>
@@ -13265,23 +13265,23 @@
     </row>
     <row r="22" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A22" s="74" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B22" s="138" t="str">
         <f>+VLOOKUP(A22,dataset!A22:B39,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C22" s="80" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D22" s="125" t="s">
         <v>1040</v>
       </c>
-      <c r="D22" s="125" t="s">
-        <v>1041</v>
-      </c>
       <c r="E22" s="125" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F22" s="87" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="G22" s="79" t="s">
         <v>47</v>
@@ -13298,23 +13298,23 @@
     </row>
     <row r="23" spans="1:14" s="117" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A23" s="74" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B23" s="138" t="str">
         <f>+VLOOKUP(A23,dataset!A23:B40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C23" s="80" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D23" s="125" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E23" s="125" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F23" s="87" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="G23" s="79" t="s">
         <v>47</v>
@@ -13331,23 +13331,23 @@
     </row>
     <row r="24" spans="1:14" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A24" s="74" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B24" s="138" t="str">
         <f>+VLOOKUP(A24,dataset!A24:B41,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C24" s="80" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D24" s="125" t="s">
         <v>1108</v>
       </c>
-      <c r="D24" s="125" t="s">
-        <v>1109</v>
-      </c>
       <c r="E24" s="125" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="F24" s="87" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="G24" s="79" t="s">
         <v>47</v>
@@ -13364,23 +13364,23 @@
     </row>
     <row r="25" spans="1:14" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A25" s="74" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B25" s="138" t="str">
         <f>+VLOOKUP(A25,dataset!A25:B42,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C25" s="80" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D25" s="125" t="s">
         <v>1185</v>
       </c>
-      <c r="D25" s="125" t="s">
+      <c r="E25" s="125" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F25" s="87" t="s">
         <v>1186</v>
-      </c>
-      <c r="E25" s="125" t="s">
-        <v>1186</v>
-      </c>
-      <c r="F25" s="87" t="s">
-        <v>1187</v>
       </c>
       <c r="G25" s="79" t="s">
         <v>47</v>
@@ -13397,23 +13397,23 @@
     </row>
     <row r="26" spans="1:14" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A26" s="74" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B26" s="138" t="str">
         <f>+VLOOKUP(A26,dataset!A26:B43,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C26" s="80" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D26" s="125" t="s">
         <v>1219</v>
       </c>
-      <c r="D26" s="125" t="s">
+      <c r="E26" s="125" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F26" s="87" t="s">
         <v>1220</v>
-      </c>
-      <c r="E26" s="125" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F26" s="87" t="s">
-        <v>1221</v>
       </c>
       <c r="G26" s="79" t="s">
         <v>47</v>
@@ -13473,7 +13473,7 @@
   </sheetPr>
   <dimension ref="A1:J561"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A553" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E14" sqref="E14"/>
       <selection pane="bottomLeft" activeCell="D556" sqref="D556"/>
@@ -15724,13 +15724,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E82" s="157" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="F82" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G82" s="153" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="H82" s="153" t="s">
         <v>389</v>
@@ -15752,13 +15752,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E83" s="157" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F83" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G83" s="153" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="H83" s="153" t="s">
         <v>400</v>
@@ -15780,13 +15780,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E84" s="157" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F84" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G84" s="153" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="H84" s="153" t="s">
         <v>391</v>
@@ -15808,13 +15808,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E85" s="157" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F85" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G85" s="153" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="H85" s="153" t="s">
         <v>391</v>
@@ -15836,13 +15836,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E86" s="157" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F86" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G86" s="153" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="H86" s="153" t="s">
         <v>391</v>
@@ -15864,13 +15864,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E87" s="157" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F87" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G87" s="153" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="H87" s="153" t="s">
         <v>389</v>
@@ -15892,13 +15892,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E88" s="157" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F88" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G88" s="153" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="H88" s="153" t="s">
         <v>389</v>
@@ -15920,13 +15920,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E89" s="157" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F89" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G89" s="153" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="H89" s="153" t="s">
         <v>389</v>
@@ -15948,13 +15948,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E90" s="157" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F90" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G90" s="153" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="H90" s="153" t="s">
         <v>400</v>
@@ -15976,13 +15976,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E91" s="157" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F91" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G91" s="153" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="H91" s="153" t="s">
         <v>400</v>
@@ -16004,13 +16004,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E92" s="157" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F92" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G92" s="153" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="H92" s="153" t="s">
         <v>399</v>
@@ -16032,13 +16032,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E93" s="157" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F93" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G93" s="153" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="H93" s="153" t="s">
         <v>395</v>
@@ -16060,13 +16060,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E94" s="157" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="F94" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G94" s="153" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="H94" s="153" t="s">
         <v>399</v>
@@ -16088,13 +16088,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E95" s="157" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="F95" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G95" s="153" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="H95" s="153" t="s">
         <v>395</v>
@@ -16116,13 +16116,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E96" s="157" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F96" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G96" s="153" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="H96" s="153" t="s">
         <v>408</v>
@@ -16144,13 +16144,13 @@
         <v>Indicadores de Hidrocarburos en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E97" s="157" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F97" s="157" t="s">
         <v>10</v>
       </c>
       <c r="G97" s="153" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="H97" s="153" t="s">
         <v>409</v>
@@ -25282,14 +25282,14 @@
     </row>
     <row r="429" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A429" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B429" s="118" t="str">
         <f>+VLOOKUP(A429,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C429" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D429" s="125" t="str">
         <f>+VLOOKUP(C429,distribution!C$2:D$40,2,FALSE)</f>
@@ -25308,14 +25308,14 @@
     </row>
     <row r="430" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A430" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B430" s="118" t="str">
         <f>+VLOOKUP(A430,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C430" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D430" s="125" t="str">
         <f>+VLOOKUP(C430,distribution!C$2:D$40,2,FALSE)</f>
@@ -25334,14 +25334,14 @@
     </row>
     <row r="431" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A431" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B431" s="118" t="str">
         <f>+VLOOKUP(A431,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C431" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D431" s="125" t="str">
         <f>+VLOOKUP(C431,distribution!C$2:D$40,2,FALSE)</f>
@@ -25360,14 +25360,14 @@
     </row>
     <row r="432" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A432" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B432" s="118" t="str">
         <f>+VLOOKUP(A432,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C432" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D432" s="125" t="str">
         <f>+VLOOKUP(C432,distribution!C$2:D$40,2,FALSE)</f>
@@ -25386,14 +25386,14 @@
     </row>
     <row r="433" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A433" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B433" s="118" t="str">
         <f>+VLOOKUP(A433,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C433" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D433" s="125" t="str">
         <f>+VLOOKUP(C433,distribution!C$2:D$40,2,FALSE)</f>
@@ -25412,27 +25412,27 @@
     </row>
     <row r="434" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A434" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B434" s="118" t="str">
         <f>+VLOOKUP(A434,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C434" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D434" s="125" t="str">
         <f>+VLOOKUP(C434,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cárnica - Porcina en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E434" s="125" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F434" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="G434" s="118" t="s">
         <v>1026</v>
-      </c>
-      <c r="F434" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="G434" s="118" t="s">
-        <v>1027</v>
       </c>
       <c r="H434" s="118" t="s">
         <v>397</v>
@@ -25440,27 +25440,27 @@
     </row>
     <row r="435" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A435" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B435" s="118" t="str">
         <f>+VLOOKUP(A435,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C435" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D435" s="125" t="str">
         <f>+VLOOKUP(C435,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cárnica - Porcina en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E435" s="125" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F435" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="G435" s="118" t="s">
         <v>1028</v>
-      </c>
-      <c r="F435" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="G435" s="118" t="s">
-        <v>1029</v>
       </c>
       <c r="H435" s="118" t="s">
         <v>397</v>
@@ -25468,55 +25468,55 @@
     </row>
     <row r="436" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A436" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B436" s="118" t="str">
         <f>+VLOOKUP(A436,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C436" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D436" s="125" t="str">
         <f>+VLOOKUP(C436,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cárnica - Porcina en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E436" s="125" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F436" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="G436" s="125" t="s">
         <v>1030</v>
       </c>
-      <c r="F436" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="G436" s="125" t="s">
-        <v>1031</v>
-      </c>
       <c r="H436" s="97" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="437" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A437" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B437" s="118" t="str">
         <f>+VLOOKUP(A437,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C437" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D437" s="125" t="str">
         <f>+VLOOKUP(C437,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cárnica - Porcina en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E437" s="125" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F437" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="G437" s="118" t="s">
         <v>1032</v>
-      </c>
-      <c r="F437" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="G437" s="118" t="s">
-        <v>1033</v>
       </c>
       <c r="H437" s="118" t="s">
         <v>416</v>
@@ -25524,42 +25524,42 @@
     </row>
     <row r="438" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A438" s="88" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B438" s="118" t="str">
         <f>+VLOOKUP(A438,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cárnica - Porcina</v>
       </c>
       <c r="C438" s="125" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D438" s="125" t="str">
         <f>+VLOOKUP(C438,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cárnica - Porcina en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E438" s="125" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F438" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="G438" s="125" t="s">
         <v>1034</v>
       </c>
-      <c r="F438" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="G438" s="125" t="s">
-        <v>1035</v>
-      </c>
       <c r="H438" s="97" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="439" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A439" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B439" s="118" t="str">
         <f>+VLOOKUP(A439,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C439" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D439" s="125" t="str">
         <f>+VLOOKUP(C439,distribution!C$2:D$40,2,FALSE)</f>
@@ -25578,14 +25578,14 @@
     </row>
     <row r="440" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A440" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B440" s="118" t="str">
         <f>+VLOOKUP(A440,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C440" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D440" s="125" t="str">
         <f>+VLOOKUP(C440,distribution!C$2:D$40,2,FALSE)</f>
@@ -25598,20 +25598,20 @@
         <v>527</v>
       </c>
       <c r="G440" s="118" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="H440" s="126"/>
     </row>
     <row r="441" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A441" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B441" s="118" t="str">
         <f>+VLOOKUP(A441,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C441" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D441" s="125" t="str">
         <f>+VLOOKUP(C441,distribution!C$2:D$40,2,FALSE)</f>
@@ -25630,14 +25630,14 @@
     </row>
     <row r="442" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A442" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B442" s="118" t="str">
         <f>+VLOOKUP(A442,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C442" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D442" s="125" t="str">
         <f>+VLOOKUP(C442,distribution!C$2:D$40,2,FALSE)</f>
@@ -25656,14 +25656,14 @@
     </row>
     <row r="443" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A443" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B443" s="118" t="str">
         <f>+VLOOKUP(A443,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C443" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D443" s="125" t="str">
         <f>+VLOOKUP(C443,distribution!C$2:D$40,2,FALSE)</f>
@@ -25682,27 +25682,27 @@
     </row>
     <row r="444" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A444" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B444" s="118" t="str">
         <f>+VLOOKUP(A444,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C444" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D444" s="125" t="str">
         <f>+VLOOKUP(C444,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E444" s="125" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F444" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G444" s="118" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="H444" s="118" t="s">
         <v>386</v>
@@ -25710,27 +25710,27 @@
     </row>
     <row r="445" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A445" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B445" s="118" t="str">
         <f>+VLOOKUP(A445,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C445" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D445" s="125" t="str">
         <f>+VLOOKUP(C445,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E445" s="125" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F445" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G445" s="118" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="H445" s="118" t="s">
         <v>386</v>
@@ -25738,27 +25738,27 @@
     </row>
     <row r="446" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A446" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B446" s="118" t="str">
         <f>+VLOOKUP(A446,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C446" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D446" s="125" t="str">
         <f>+VLOOKUP(C446,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E446" s="125" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F446" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G446" s="118" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="H446" s="118" t="s">
         <v>393</v>
@@ -25766,27 +25766,27 @@
     </row>
     <row r="447" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A447" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B447" s="118" t="str">
         <f>+VLOOKUP(A447,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C447" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D447" s="125" t="str">
         <f>+VLOOKUP(C447,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E447" s="125" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F447" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G447" s="118" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="H447" s="118" t="s">
         <v>393</v>
@@ -25794,27 +25794,27 @@
     </row>
     <row r="448" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A448" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B448" s="118" t="str">
         <f>+VLOOKUP(A448,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C448" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D448" s="125" t="str">
         <f>+VLOOKUP(C448,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E448" s="125" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="F448" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G448" s="118" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="H448" s="118" t="s">
         <v>393</v>
@@ -25822,27 +25822,27 @@
     </row>
     <row r="449" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A449" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B449" s="118" t="str">
         <f>+VLOOKUP(A449,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C449" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D449" s="125" t="str">
         <f>+VLOOKUP(C449,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E449" s="125" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="F449" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G449" s="118" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="H449" s="118" t="s">
         <v>393</v>
@@ -25850,27 +25850,27 @@
     </row>
     <row r="450" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A450" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B450" s="118" t="str">
         <f>+VLOOKUP(A450,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C450" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D450" s="125" t="str">
         <f>+VLOOKUP(C450,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E450" s="125" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F450" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G450" s="118" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="H450" s="118" t="s">
         <v>393</v>
@@ -25878,27 +25878,27 @@
     </row>
     <row r="451" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A451" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B451" s="118" t="str">
         <f>+VLOOKUP(A451,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C451" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D451" s="125" t="str">
         <f>+VLOOKUP(C451,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E451" s="125" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F451" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G451" s="118" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="H451" s="118" t="s">
         <v>393</v>
@@ -25906,27 +25906,27 @@
     </row>
     <row r="452" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A452" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B452" s="118" t="str">
         <f>+VLOOKUP(A452,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C452" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D452" s="125" t="str">
         <f>+VLOOKUP(C452,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E452" s="125" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F452" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G452" s="118" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="H452" s="118" t="s">
         <v>393</v>
@@ -25934,27 +25934,27 @@
     </row>
     <row r="453" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A453" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B453" s="118" t="str">
         <f>+VLOOKUP(A453,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C453" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D453" s="125" t="str">
         <f>+VLOOKUP(C453,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E453" s="125" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="F453" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G453" s="118" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="H453" s="118" t="s">
         <v>393</v>
@@ -25962,27 +25962,27 @@
     </row>
     <row r="454" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A454" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B454" s="118" t="str">
         <f>+VLOOKUP(A454,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C454" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D454" s="125" t="str">
         <f>+VLOOKUP(C454,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E454" s="125" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="F454" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G454" s="118" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="H454" s="118" t="s">
         <v>416</v>
@@ -25990,27 +25990,27 @@
     </row>
     <row r="455" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A455" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B455" s="118" t="str">
         <f>+VLOOKUP(A455,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C455" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D455" s="125" t="str">
         <f>+VLOOKUP(C455,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E455" s="125" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="F455" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G455" s="118" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="H455" s="118" t="s">
         <v>416</v>
@@ -26018,27 +26018,27 @@
     </row>
     <row r="456" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A456" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B456" s="118" t="str">
         <f>+VLOOKUP(A456,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C456" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D456" s="125" t="str">
         <f>+VLOOKUP(C456,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E456" s="125" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="F456" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G456" s="118" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="H456" s="118" t="s">
         <v>393</v>
@@ -26046,27 +26046,27 @@
     </row>
     <row r="457" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A457" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B457" s="118" t="str">
         <f>+VLOOKUP(A457,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C457" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D457" s="125" t="str">
         <f>+VLOOKUP(C457,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E457" s="125" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="F457" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G457" s="118" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="H457" s="118" t="s">
         <v>393</v>
@@ -26074,27 +26074,27 @@
     </row>
     <row r="458" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A458" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B458" s="118" t="str">
         <f>+VLOOKUP(A458,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C458" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D458" s="125" t="str">
         <f>+VLOOKUP(C458,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E458" s="125" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="F458" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G458" s="118" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="H458" s="118" t="s">
         <v>393</v>
@@ -26102,27 +26102,27 @@
     </row>
     <row r="459" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A459" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B459" s="118" t="str">
         <f>+VLOOKUP(A459,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C459" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D459" s="125" t="str">
         <f>+VLOOKUP(C459,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E459" s="125" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="F459" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G459" s="118" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="H459" s="118" t="s">
         <v>393</v>
@@ -26130,27 +26130,27 @@
     </row>
     <row r="460" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A460" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B460" s="118" t="str">
         <f>+VLOOKUP(A460,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C460" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D460" s="125" t="str">
         <f>+VLOOKUP(C460,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E460" s="125" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F460" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G460" s="118" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H460" s="118" t="s">
         <v>393</v>
@@ -26158,27 +26158,27 @@
     </row>
     <row r="461" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A461" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B461" s="118" t="str">
         <f>+VLOOKUP(A461,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C461" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D461" s="125" t="str">
         <f>+VLOOKUP(C461,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E461" s="125" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="F461" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G461" s="118" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="H461" s="118" t="s">
         <v>393</v>
@@ -26186,27 +26186,27 @@
     </row>
     <row r="462" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A462" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B462" s="118" t="str">
         <f>+VLOOKUP(A462,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C462" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D462" s="125" t="str">
         <f>+VLOOKUP(C462,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E462" s="125" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="F462" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G462" s="118" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="H462" s="118" t="s">
         <v>403</v>
@@ -26214,27 +26214,27 @@
     </row>
     <row r="463" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A463" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B463" s="118" t="str">
         <f>+VLOOKUP(A463,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Cítricos dulces</v>
       </c>
       <c r="C463" s="125" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D463" s="125" t="str">
         <f>+VLOOKUP(C463,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Cítricos dulces en valores anuales y mensuales</v>
       </c>
       <c r="E463" s="125" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F463" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G463" s="118" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="H463" s="118" t="s">
         <v>403</v>
@@ -26242,14 +26242,14 @@
     </row>
     <row r="464" spans="1:8" s="123" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A464" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B464" s="118" t="str">
         <f>+VLOOKUP(A464,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C464" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D464" s="125" t="str">
         <f>+VLOOKUP(C464,distribution!C$2:D$40,2,FALSE)</f>
@@ -26268,14 +26268,14 @@
     </row>
     <row r="465" spans="1:8" s="123" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A465" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B465" s="118" t="str">
         <f>+VLOOKUP(A465,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C465" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D465" s="125" t="str">
         <f>+VLOOKUP(C465,distribution!C$2:D$40,2,FALSE)</f>
@@ -26288,20 +26288,20 @@
         <v>527</v>
       </c>
       <c r="G465" s="118" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="H465" s="126"/>
     </row>
     <row r="466" spans="1:8" s="123" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A466" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B466" s="118" t="str">
         <f>+VLOOKUP(A466,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C466" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D466" s="125" t="str">
         <f>+VLOOKUP(C466,distribution!C$2:D$40,2,FALSE)</f>
@@ -26320,14 +26320,14 @@
     </row>
     <row r="467" spans="1:8" s="123" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A467" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B467" s="118" t="str">
         <f>+VLOOKUP(A467,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C467" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D467" s="125" t="str">
         <f>+VLOOKUP(C467,distribution!C$2:D$40,2,FALSE)</f>
@@ -26346,14 +26346,14 @@
     </row>
     <row r="468" spans="1:8" s="123" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A468" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B468" s="118" t="str">
         <f>+VLOOKUP(A468,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C468" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D468" s="125" t="str">
         <f>+VLOOKUP(C468,distribution!C$2:D$40,2,FALSE)</f>
@@ -26372,27 +26372,27 @@
     </row>
     <row r="469" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A469" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B469" s="118" t="str">
         <f>+VLOOKUP(A469,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C469" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D469" s="125" t="str">
         <f>+VLOOKUP(C469,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Construcción en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E469" s="125" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F469" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G469" s="118" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="H469" s="97" t="s">
         <v>393</v>
@@ -26400,27 +26400,27 @@
     </row>
     <row r="470" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A470" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B470" s="118" t="str">
         <f>+VLOOKUP(A470,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C470" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D470" s="125" t="str">
         <f>+VLOOKUP(C470,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Construcción en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E470" s="125" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="F470" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G470" s="118" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="H470" s="97" t="s">
         <v>384</v>
@@ -26428,55 +26428,55 @@
     </row>
     <row r="471" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A471" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B471" s="118" t="str">
         <f>+VLOOKUP(A471,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C471" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D471" s="125" t="str">
         <f>+VLOOKUP(C471,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Construcción en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E471" s="125" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F471" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G471" s="118" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="H471" s="97" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="472" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A472" s="88" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B472" s="118" t="str">
         <f>+VLOOKUP(A472,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Construcción</v>
       </c>
       <c r="C472" s="125" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D472" s="125" t="str">
         <f>+VLOOKUP(C472,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Construcción en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E472" s="125" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F472" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G472" s="118" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H472" s="97" t="s">
         <v>401</v>
@@ -26484,14 +26484,14 @@
     </row>
     <row r="473" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A473" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B473" s="118" t="str">
         <f>+VLOOKUP(A473,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C473" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D473" s="125" t="str">
         <f>+VLOOKUP(C473,distribution!C$2:D$40,2,FALSE)</f>
@@ -26510,14 +26510,14 @@
     </row>
     <row r="474" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A474" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B474" s="118" t="str">
         <f>+VLOOKUP(A474,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C474" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D474" s="125" t="str">
         <f>+VLOOKUP(C474,distribution!C$2:D$40,2,FALSE)</f>
@@ -26530,20 +26530,20 @@
         <v>527</v>
       </c>
       <c r="G474" s="118" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="H474" s="126"/>
     </row>
     <row r="475" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A475" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B475" s="118" t="str">
         <f>+VLOOKUP(A475,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C475" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D475" s="125" t="str">
         <f>+VLOOKUP(C475,distribution!C$2:D$40,2,FALSE)</f>
@@ -26562,14 +26562,14 @@
     </row>
     <row r="476" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A476" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B476" s="118" t="str">
         <f>+VLOOKUP(A476,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C476" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D476" s="125" t="str">
         <f>+VLOOKUP(C476,distribution!C$2:D$40,2,FALSE)</f>
@@ -26588,14 +26588,14 @@
     </row>
     <row r="477" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A477" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B477" s="118" t="str">
         <f>+VLOOKUP(A477,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C477" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D477" s="125" t="str">
         <f>+VLOOKUP(C477,distribution!C$2:D$40,2,FALSE)</f>
@@ -26614,27 +26614,27 @@
     </row>
     <row r="478" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A478" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B478" s="118" t="str">
         <f>+VLOOKUP(A478,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C478" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D478" s="125" t="str">
         <f>+VLOOKUP(C478,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E478" s="125" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F478" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G478" s="118" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="H478" s="118" t="s">
         <v>386</v>
@@ -26642,27 +26642,27 @@
     </row>
     <row r="479" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A479" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B479" s="118" t="str">
         <f>+VLOOKUP(A479,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C479" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D479" s="125" t="str">
         <f>+VLOOKUP(C479,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E479" s="125" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="F479" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G479" s="118" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="H479" s="118" t="s">
         <v>386</v>
@@ -26670,27 +26670,27 @@
     </row>
     <row r="480" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A480" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B480" s="118" t="str">
         <f>+VLOOKUP(A480,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C480" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D480" s="125" t="str">
         <f>+VLOOKUP(C480,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E480" s="125" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="F480" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G480" s="118" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="H480" s="118" t="s">
         <v>386</v>
@@ -26698,27 +26698,27 @@
     </row>
     <row r="481" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A481" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B481" s="118" t="str">
         <f>+VLOOKUP(A481,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C481" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D481" s="125" t="str">
         <f>+VLOOKUP(C481,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E481" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F481" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G481" s="118" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="H481" s="118" t="s">
         <v>386</v>
@@ -26726,27 +26726,27 @@
     </row>
     <row r="482" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A482" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B482" s="118" t="str">
         <f>+VLOOKUP(A482,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C482" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D482" s="125" t="str">
         <f>+VLOOKUP(C482,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E482" s="125" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F482" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G482" s="118" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="H482" s="118" t="s">
         <v>393</v>
@@ -26754,27 +26754,27 @@
     </row>
     <row r="483" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A483" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B483" s="118" t="str">
         <f>+VLOOKUP(A483,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C483" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D483" s="125" t="str">
         <f>+VLOOKUP(C483,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E483" s="125" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F483" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G483" s="118" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="H483" s="118" t="s">
         <v>393</v>
@@ -26782,27 +26782,27 @@
     </row>
     <row r="484" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A484" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B484" s="118" t="str">
         <f>+VLOOKUP(A484,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C484" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D484" s="125" t="str">
         <f>+VLOOKUP(C484,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E484" s="125" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="F484" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G484" s="118" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="H484" s="118" t="s">
         <v>393</v>
@@ -26810,27 +26810,27 @@
     </row>
     <row r="485" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A485" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B485" s="118" t="str">
         <f>+VLOOKUP(A485,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C485" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D485" s="125" t="str">
         <f>+VLOOKUP(C485,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E485" s="125" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F485" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G485" s="118" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="H485" s="118" t="s">
         <v>393</v>
@@ -26838,27 +26838,27 @@
     </row>
     <row r="486" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A486" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B486" s="118" t="str">
         <f>+VLOOKUP(A486,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C486" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D486" s="125" t="str">
         <f>+VLOOKUP(C486,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E486" s="125" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="F486" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G486" s="118" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="H486" s="118" t="s">
         <v>393</v>
@@ -26866,27 +26866,27 @@
     </row>
     <row r="487" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A487" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B487" s="118" t="str">
         <f>+VLOOKUP(A487,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C487" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D487" s="125" t="str">
         <f>+VLOOKUP(C487,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E487" s="125" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F487" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G487" s="118" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="H487" s="118" t="s">
         <v>393</v>
@@ -26894,27 +26894,27 @@
     </row>
     <row r="488" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A488" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B488" s="118" t="str">
         <f>+VLOOKUP(A488,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C488" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D488" s="125" t="str">
         <f>+VLOOKUP(C488,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E488" s="125" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="F488" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G488" s="118" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="H488" s="118" t="s">
         <v>393</v>
@@ -26922,27 +26922,27 @@
     </row>
     <row r="489" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A489" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B489" s="118" t="str">
         <f>+VLOOKUP(A489,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C489" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D489" s="125" t="str">
         <f>+VLOOKUP(C489,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E489" s="125" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="F489" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G489" s="118" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="H489" s="118" t="s">
         <v>393</v>
@@ -26950,27 +26950,27 @@
     </row>
     <row r="490" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A490" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B490" s="118" t="str">
         <f>+VLOOKUP(A490,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C490" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D490" s="125" t="str">
         <f>+VLOOKUP(C490,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E490" s="125" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="F490" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G490" s="118" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="H490" s="118" t="s">
         <v>393</v>
@@ -26978,27 +26978,27 @@
     </row>
     <row r="491" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A491" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B491" s="118" t="str">
         <f>+VLOOKUP(A491,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C491" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D491" s="125" t="str">
         <f>+VLOOKUP(C491,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E491" s="125" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="F491" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G491" s="118" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="H491" s="118" t="s">
         <v>393</v>
@@ -27006,27 +27006,27 @@
     </row>
     <row r="492" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A492" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B492" s="118" t="str">
         <f>+VLOOKUP(A492,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C492" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D492" s="125" t="str">
         <f>+VLOOKUP(C492,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E492" s="125" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="F492" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G492" s="118" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="H492" s="118" t="s">
         <v>393</v>
@@ -27034,27 +27034,27 @@
     </row>
     <row r="493" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A493" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B493" s="118" t="str">
         <f>+VLOOKUP(A493,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C493" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D493" s="125" t="str">
         <f>+VLOOKUP(C493,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E493" s="125" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="F493" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G493" s="118" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="H493" s="118" t="s">
         <v>414</v>
@@ -27062,27 +27062,27 @@
     </row>
     <row r="494" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A494" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B494" s="118" t="str">
         <f>+VLOOKUP(A494,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C494" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D494" s="125" t="str">
         <f>+VLOOKUP(C494,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E494" s="125" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="F494" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G494" s="118" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="H494" s="118" t="s">
         <v>414</v>
@@ -27090,27 +27090,27 @@
     </row>
     <row r="495" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A495" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B495" s="118" t="str">
         <f>+VLOOKUP(A495,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C495" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D495" s="125" t="str">
         <f>+VLOOKUP(C495,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E495" s="125" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="F495" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G495" s="118" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="H495" s="118" t="s">
         <v>414</v>
@@ -27118,27 +27118,27 @@
     </row>
     <row r="496" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A496" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B496" s="118" t="str">
         <f>+VLOOKUP(A496,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C496" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D496" s="125" t="str">
         <f>+VLOOKUP(C496,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E496" s="125" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="F496" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G496" s="118" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="H496" s="118" t="s">
         <v>414</v>
@@ -27146,27 +27146,27 @@
     </row>
     <row r="497" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A497" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B497" s="118" t="str">
         <f>+VLOOKUP(A497,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C497" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D497" s="125" t="str">
         <f>+VLOOKUP(C497,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E497" s="125" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="F497" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G497" s="118" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="H497" s="118" t="s">
         <v>414</v>
@@ -27174,27 +27174,27 @@
     </row>
     <row r="498" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A498" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B498" s="118" t="str">
         <f>+VLOOKUP(A498,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C498" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D498" s="125" t="str">
         <f>+VLOOKUP(C498,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E498" s="125" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F498" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G498" s="118" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="H498" s="118" t="s">
         <v>414</v>
@@ -27202,27 +27202,27 @@
     </row>
     <row r="499" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A499" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B499" s="118" t="str">
         <f>+VLOOKUP(A499,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C499" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D499" s="125" t="str">
         <f>+VLOOKUP(C499,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E499" s="125" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F499" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G499" s="118" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="H499" s="118" t="s">
         <v>414</v>
@@ -27230,27 +27230,27 @@
     </row>
     <row r="500" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A500" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B500" s="118" t="str">
         <f>+VLOOKUP(A500,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C500" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D500" s="125" t="str">
         <f>+VLOOKUP(C500,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E500" s="125" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F500" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G500" s="118" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="H500" s="118" t="s">
         <v>414</v>
@@ -27258,27 +27258,27 @@
     </row>
     <row r="501" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A501" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B501" s="118" t="str">
         <f>+VLOOKUP(A501,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C501" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D501" s="125" t="str">
         <f>+VLOOKUP(C501,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E501" s="125" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F501" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G501" s="118" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="H501" s="118" t="s">
         <v>414</v>
@@ -27286,27 +27286,27 @@
     </row>
     <row r="502" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A502" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B502" s="118" t="str">
         <f>+VLOOKUP(A502,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C502" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D502" s="125" t="str">
         <f>+VLOOKUP(C502,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E502" s="125" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F502" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G502" s="118" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="H502" s="118" t="s">
         <v>414</v>
@@ -27314,27 +27314,27 @@
     </row>
     <row r="503" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A503" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B503" s="118" t="str">
         <f>+VLOOKUP(A503,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C503" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D503" s="125" t="str">
         <f>+VLOOKUP(C503,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E503" s="125" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F503" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G503" s="118" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="H503" s="118" t="s">
         <v>413</v>
@@ -27342,27 +27342,27 @@
     </row>
     <row r="504" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A504" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B504" s="118" t="str">
         <f>+VLOOKUP(A504,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C504" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D504" s="125" t="str">
         <f>+VLOOKUP(C504,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E504" s="125" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F504" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G504" s="118" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="H504" s="118" t="s">
         <v>413</v>
@@ -27370,27 +27370,27 @@
     </row>
     <row r="505" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A505" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B505" s="118" t="str">
         <f>+VLOOKUP(A505,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C505" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D505" s="125" t="str">
         <f>+VLOOKUP(C505,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E505" s="125" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F505" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G505" s="118" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="H505" s="118" t="s">
         <v>413</v>
@@ -27398,27 +27398,27 @@
     </row>
     <row r="506" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A506" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B506" s="118" t="str">
         <f>+VLOOKUP(A506,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C506" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D506" s="125" t="str">
         <f>+VLOOKUP(C506,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E506" s="125" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F506" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G506" s="118" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="H506" s="118" t="s">
         <v>413</v>
@@ -27426,27 +27426,27 @@
     </row>
     <row r="507" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A507" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B507" s="118" t="str">
         <f>+VLOOKUP(A507,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C507" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D507" s="125" t="str">
         <f>+VLOOKUP(C507,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E507" s="125" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F507" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G507" s="118" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="H507" s="118" t="s">
         <v>413</v>
@@ -27454,27 +27454,27 @@
     </row>
     <row r="508" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A508" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B508" s="118" t="str">
         <f>+VLOOKUP(A508,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C508" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D508" s="125" t="str">
         <f>+VLOOKUP(C508,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E508" s="125" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F508" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G508" s="118" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="H508" s="118" t="s">
         <v>413</v>
@@ -27482,27 +27482,27 @@
     </row>
     <row r="509" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A509" s="88" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B509" s="118" t="str">
         <f>+VLOOKUP(A509,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Oleaginosa</v>
       </c>
       <c r="C509" s="125" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D509" s="125" t="str">
         <f>+VLOOKUP(C509,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Oleaginosa en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E509" s="125" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="F509" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G509" s="118" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="H509" s="118" t="s">
         <v>413</v>
@@ -27510,14 +27510,14 @@
     </row>
     <row r="510" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A510" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B510" s="118" t="str">
         <f>+VLOOKUP(A510,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C510" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D510" s="125" t="str">
         <f>+VLOOKUP(C510,distribution!C$2:D$40,2,FALSE)</f>
@@ -27536,14 +27536,14 @@
     </row>
     <row r="511" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A511" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B511" s="118" t="str">
         <f>+VLOOKUP(A511,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C511" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D511" s="125" t="str">
         <f>+VLOOKUP(C511,distribution!C$2:D$40,2,FALSE)</f>
@@ -27556,20 +27556,20 @@
         <v>527</v>
       </c>
       <c r="G511" s="118" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="H511" s="89"/>
     </row>
     <row r="512" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A512" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B512" s="118" t="str">
         <f>+VLOOKUP(A512,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C512" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D512" s="125" t="str">
         <f>+VLOOKUP(C512,distribution!C$2:D$40,2,FALSE)</f>
@@ -27588,14 +27588,14 @@
     </row>
     <row r="513" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A513" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B513" s="118" t="str">
         <f>+VLOOKUP(A513,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C513" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D513" s="125" t="str">
         <f>+VLOOKUP(C513,distribution!C$2:D$40,2,FALSE)</f>
@@ -27614,14 +27614,14 @@
     </row>
     <row r="514" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A514" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B514" s="118" t="str">
         <f>+VLOOKUP(A514,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C514" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D514" s="125" t="str">
         <f>+VLOOKUP(C514,distribution!C$2:D$40,2,FALSE)</f>
@@ -27640,27 +27640,27 @@
     </row>
     <row r="515" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A515" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B515" s="118" t="str">
         <f>+VLOOKUP(A515,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C515" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D515" s="125" t="str">
         <f>+VLOOKUP(C515,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E515" s="125" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="F515" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G515" s="118" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="H515" s="89" t="s">
         <v>397</v>
@@ -27669,27 +27669,27 @@
     </row>
     <row r="516" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A516" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B516" s="118" t="str">
         <f>+VLOOKUP(A516,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C516" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D516" s="125" t="str">
         <f>+VLOOKUP(C516,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E516" s="125" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="F516" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G516" s="118" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="H516" s="89" t="s">
         <v>397</v>
@@ -27698,114 +27698,114 @@
     </row>
     <row r="517" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A517" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B517" s="118" t="str">
         <f>+VLOOKUP(A517,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C517" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D517" s="125" t="str">
         <f>+VLOOKUP(C517,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E517" s="125" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="F517" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G517" s="118" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="H517" s="89" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="I517" s="184"/>
     </row>
     <row r="518" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A518" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B518" s="118" t="str">
         <f>+VLOOKUP(A518,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C518" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D518" s="125" t="str">
         <f>+VLOOKUP(C518,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E518" s="125" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="F518" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G518" s="118" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="H518" s="89" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="I518" s="184"/>
     </row>
     <row r="519" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A519" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B519" s="118" t="str">
         <f>+VLOOKUP(A519,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C519" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D519" s="125" t="str">
         <f>+VLOOKUP(C519,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E519" s="125" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F519" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G519" s="118" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="H519" s="89" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="I519" s="184"/>
     </row>
     <row r="520" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A520" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B520" s="118" t="str">
         <f>+VLOOKUP(A520,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C520" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D520" s="125" t="str">
         <f>+VLOOKUP(C520,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E520" s="125" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="F520" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G520" s="118" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="H520" s="89" t="s">
         <v>416</v>
@@ -27814,27 +27814,27 @@
     </row>
     <row r="521" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A521" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B521" s="118" t="str">
         <f>+VLOOKUP(A521,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C521" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D521" s="125" t="str">
         <f>+VLOOKUP(C521,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E521" s="125" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="F521" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G521" s="118" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="H521" s="89" t="s">
         <v>393</v>
@@ -27843,27 +27843,27 @@
     </row>
     <row r="522" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A522" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B522" s="118" t="str">
         <f>+VLOOKUP(A522,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C522" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D522" s="125" t="str">
         <f>+VLOOKUP(C522,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E522" s="125" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="F522" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G522" s="118" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="H522" s="89" t="s">
         <v>393</v>
@@ -27872,27 +27872,27 @@
     </row>
     <row r="523" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A523" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B523" s="118" t="str">
         <f>+VLOOKUP(A523,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C523" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D523" s="125" t="str">
         <f>+VLOOKUP(C523,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E523" s="125" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="F523" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G523" s="118" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="H523" s="89" t="s">
         <v>393</v>
@@ -27901,27 +27901,27 @@
     </row>
     <row r="524" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A524" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B524" s="118" t="str">
         <f>+VLOOKUP(A524,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C524" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D524" s="125" t="str">
         <f>+VLOOKUP(C524,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E524" s="125" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="F524" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G524" s="118" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="H524" s="89" t="s">
         <v>393</v>
@@ -27930,27 +27930,27 @@
     </row>
     <row r="525" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A525" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B525" s="118" t="str">
         <f>+VLOOKUP(A525,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C525" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D525" s="125" t="str">
         <f>+VLOOKUP(C525,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E525" s="125" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="F525" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G525" s="118" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="H525" s="89" t="s">
         <v>393</v>
@@ -27959,27 +27959,27 @@
     </row>
     <row r="526" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A526" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B526" s="118" t="str">
         <f>+VLOOKUP(A526,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C526" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D526" s="125" t="str">
         <f>+VLOOKUP(C526,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E526" s="125" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="F526" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G526" s="118" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="H526" s="89" t="s">
         <v>395</v>
@@ -27987,27 +27987,27 @@
     </row>
     <row r="527" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A527" s="88" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B527" s="118" t="str">
         <f>+VLOOKUP(A527,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Ovinos - Lana y Carne</v>
       </c>
       <c r="C527" s="125" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D527" s="125" t="str">
         <f>+VLOOKUP(C527,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Ovinos - Lana y Carne en valores anuales y mensuales</v>
       </c>
       <c r="E527" s="125" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="F527" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G527" s="118" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="H527" s="89" t="s">
         <v>395</v>
@@ -28015,14 +28015,14 @@
     </row>
     <row r="528" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A528" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B528" s="118" t="str">
         <f>+VLOOKUP(A528,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C528" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D528" s="125" t="str">
         <f>+VLOOKUP(C528,distribution!C$2:D$40,2,FALSE)</f>
@@ -28035,7 +28035,7 @@
         <v>9</v>
       </c>
       <c r="G528" s="118" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H528" s="89"/>
       <c r="I528" s="123"/>
@@ -28043,14 +28043,14 @@
     </row>
     <row r="529" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A529" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B529" s="118" t="str">
         <f>+VLOOKUP(A529,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C529" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D529" s="125" t="str">
         <f>+VLOOKUP(C529,distribution!C$2:D$40,2,FALSE)</f>
@@ -28071,14 +28071,14 @@
     </row>
     <row r="530" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A530" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B530" s="118" t="str">
         <f>+VLOOKUP(A530,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C530" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D530" s="125" t="str">
         <f>+VLOOKUP(C530,distribution!C$2:D$40,2,FALSE)</f>
@@ -28099,14 +28099,14 @@
     </row>
     <row r="531" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A531" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B531" s="118" t="str">
         <f>+VLOOKUP(A531,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C531" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D531" s="125" t="str">
         <f>+VLOOKUP(C531,distribution!C$2:D$40,2,FALSE)</f>
@@ -28127,14 +28127,14 @@
     </row>
     <row r="532" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A532" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B532" s="118" t="str">
         <f>+VLOOKUP(A532,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C532" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D532" s="125" t="str">
         <f>+VLOOKUP(C532,distribution!C$2:D$40,2,FALSE)</f>
@@ -28155,27 +28155,27 @@
     </row>
     <row r="533" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A533" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B533" s="118" t="str">
         <f>+VLOOKUP(A533,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C533" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D533" s="125" t="str">
         <f>+VLOOKUP(C533,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E533" s="125" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="F533" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G533" s="118" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="H533" s="89" t="s">
         <v>384</v>
@@ -28185,57 +28185,57 @@
     </row>
     <row r="534" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A534" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B534" s="118" t="str">
         <f>+VLOOKUP(A534,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C534" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D534" s="125" t="str">
         <f>+VLOOKUP(C534,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E534" s="125" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="F534" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G534" s="118" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="H534" s="89" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="I534" s="185"/>
       <c r="J534" s="123"/>
     </row>
     <row r="535" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A535" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B535" s="118" t="str">
         <f>+VLOOKUP(A535,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C535" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D535" s="125" t="str">
         <f>+VLOOKUP(C535,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E535" s="125" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="F535" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G535" s="118" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="H535" s="89" t="s">
         <v>384</v>
@@ -28245,777 +28245,777 @@
     </row>
     <row r="536" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A536" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B536" s="118" t="str">
         <f>+VLOOKUP(A536,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C536" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D536" s="125" t="str">
         <f>+VLOOKUP(C536,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E536" s="125" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="F536" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G536" s="118" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="H536" s="89" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="I536" s="185"/>
       <c r="J536" s="123"/>
     </row>
     <row r="537" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A537" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B537" s="118" t="str">
         <f>+VLOOKUP(A537,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C537" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D537" s="125" t="str">
         <f>+VLOOKUP(C537,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E537" s="125" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="F537" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G537" s="118" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="H537" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I537" s="185"/>
       <c r="J537" s="123"/>
     </row>
     <row r="538" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A538" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B538" s="118" t="str">
         <f>+VLOOKUP(A538,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C538" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D538" s="125" t="str">
         <f>+VLOOKUP(C538,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E538" s="125" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="F538" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G538" s="118" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="H538" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I538" s="185"/>
       <c r="J538" s="123"/>
     </row>
     <row r="539" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A539" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B539" s="118" t="str">
         <f>+VLOOKUP(A539,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C539" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D539" s="125" t="str">
         <f>+VLOOKUP(C539,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E539" s="125" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="F539" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G539" s="118" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="H539" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I539" s="185"/>
       <c r="J539" s="123"/>
     </row>
     <row r="540" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A540" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B540" s="118" t="str">
         <f>+VLOOKUP(A540,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C540" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D540" s="125" t="str">
         <f>+VLOOKUP(C540,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E540" s="125" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F540" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G540" s="118" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="H540" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I540" s="185"/>
       <c r="J540" s="123"/>
     </row>
     <row r="541" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A541" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B541" s="118" t="str">
         <f>+VLOOKUP(A541,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C541" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D541" s="125" t="str">
         <f>+VLOOKUP(C541,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E541" s="125" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="F541" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G541" s="118" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="H541" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I541" s="185"/>
       <c r="J541" s="123"/>
     </row>
     <row r="542" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A542" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B542" s="118" t="str">
         <f>+VLOOKUP(A542,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C542" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D542" s="125" t="str">
         <f>+VLOOKUP(C542,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E542" s="125" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="F542" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G542" s="118" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="H542" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I542" s="185"/>
       <c r="J542" s="123"/>
     </row>
     <row r="543" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A543" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B543" s="118" t="str">
         <f>+VLOOKUP(A543,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C543" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D543" s="125" t="str">
         <f>+VLOOKUP(C543,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E543" s="125" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="F543" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G543" s="118" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="H543" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I543" s="185"/>
       <c r="J543" s="123"/>
     </row>
     <row r="544" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A544" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B544" s="118" t="str">
         <f>+VLOOKUP(A544,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C544" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D544" s="125" t="str">
         <f>+VLOOKUP(C544,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E544" s="125" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F544" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G544" s="118" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="H544" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I544" s="185"/>
       <c r="J544" s="123"/>
     </row>
     <row r="545" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A545" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B545" s="118" t="str">
         <f>+VLOOKUP(A545,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C545" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D545" s="125" t="str">
         <f>+VLOOKUP(C545,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E545" s="125" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="F545" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G545" s="118" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="H545" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I545" s="185"/>
       <c r="J545" s="123"/>
     </row>
     <row r="546" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A546" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B546" s="118" t="str">
         <f>+VLOOKUP(A546,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C546" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D546" s="125" t="str">
         <f>+VLOOKUP(C546,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E546" s="125" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="F546" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G546" s="118" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="H546" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I546" s="185"/>
       <c r="J546" s="123"/>
     </row>
     <row r="547" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A547" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B547" s="118" t="str">
         <f>+VLOOKUP(A547,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C547" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D547" s="125" t="str">
         <f>+VLOOKUP(C547,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E547" s="125" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="F547" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G547" s="118" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="H547" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I547" s="185"/>
       <c r="J547" s="123"/>
     </row>
     <row r="548" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A548" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B548" s="118" t="str">
         <f>+VLOOKUP(A548,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C548" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D548" s="125" t="str">
         <f>+VLOOKUP(C548,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E548" s="125" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="F548" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G548" s="118" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="H548" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I548" s="185"/>
       <c r="J548" s="123"/>
     </row>
     <row r="549" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A549" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B549" s="118" t="str">
         <f>+VLOOKUP(A549,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C549" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D549" s="125" t="str">
         <f>+VLOOKUP(C549,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E549" s="125" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="F549" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G549" s="118" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="H549" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I549" s="185"/>
       <c r="J549" s="123"/>
     </row>
     <row r="550" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A550" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B550" s="118" t="str">
         <f>+VLOOKUP(A550,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C550" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D550" s="125" t="str">
         <f>+VLOOKUP(C550,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E550" s="125" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="F550" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G550" s="118" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="H550" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I550" s="185"/>
       <c r="J550" s="123"/>
     </row>
     <row r="551" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A551" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B551" s="118" t="str">
         <f>+VLOOKUP(A551,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C551" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D551" s="125" t="str">
         <f>+VLOOKUP(C551,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E551" s="125" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="F551" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G551" s="118" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="H551" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I551" s="185"/>
       <c r="J551" s="123"/>
     </row>
     <row r="552" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A552" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B552" s="118" t="str">
         <f>+VLOOKUP(A552,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C552" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D552" s="125" t="str">
         <f>+VLOOKUP(C552,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E552" s="125" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="F552" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G552" s="118" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="H552" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I552" s="185"/>
       <c r="J552" s="123"/>
     </row>
     <row r="553" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A553" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B553" s="118" t="str">
         <f>+VLOOKUP(A553,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C553" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D553" s="125" t="str">
         <f>+VLOOKUP(C553,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E553" s="125" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="F553" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G553" s="118" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="H553" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I553" s="185"/>
       <c r="J553" s="123"/>
     </row>
     <row r="554" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A554" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B554" s="118" t="str">
         <f>+VLOOKUP(A554,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C554" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D554" s="125" t="str">
         <f>+VLOOKUP(C554,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E554" s="125" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="F554" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G554" s="118" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="H554" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I554" s="185"/>
       <c r="J554" s="123"/>
     </row>
     <row r="555" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A555" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B555" s="118" t="str">
         <f>+VLOOKUP(A555,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C555" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D555" s="125" t="str">
         <f>+VLOOKUP(C555,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E555" s="125" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="F555" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G555" s="118" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="H555" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I555" s="185"/>
       <c r="J555" s="123"/>
     </row>
     <row r="556" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A556" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B556" s="118" t="str">
         <f>+VLOOKUP(A556,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C556" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D556" s="125" t="str">
         <f>+VLOOKUP(C556,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E556" s="125" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="F556" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G556" s="118" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="H556" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I556" s="185"/>
       <c r="J556" s="123"/>
     </row>
     <row r="557" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A557" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B557" s="118" t="str">
         <f>+VLOOKUP(A557,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C557" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D557" s="125" t="str">
         <f>+VLOOKUP(C557,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E557" s="125" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="F557" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G557" s="118" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="H557" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I557" s="185"/>
       <c r="J557" s="123"/>
     </row>
     <row r="558" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A558" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B558" s="118" t="str">
         <f>+VLOOKUP(A558,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C558" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D558" s="125" t="str">
         <f>+VLOOKUP(C558,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E558" s="125" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="F558" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G558" s="118" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="H558" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I558" s="185"/>
       <c r="J558" s="123"/>
     </row>
     <row r="559" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A559" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B559" s="118" t="str">
         <f>+VLOOKUP(A559,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C559" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D559" s="125" t="str">
         <f>+VLOOKUP(C559,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E559" s="125" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="F559" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G559" s="118" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="H559" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I559" s="185"/>
       <c r="J559" s="123"/>
     </row>
     <row r="560" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A560" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B560" s="118" t="str">
         <f>+VLOOKUP(A560,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C560" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D560" s="125" t="str">
         <f>+VLOOKUP(C560,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E560" s="125" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="F560" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G560" s="118" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="H560" s="89" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I560" s="185"/>
       <c r="J560" s="123"/>
     </row>
     <row r="561" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A561" s="88" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B561" s="118" t="str">
         <f>+VLOOKUP(A561,dataset!A$2:B$40,2,FALSE)</f>
         <v>Indicadores Sectoriales de Comercio interno</v>
       </c>
       <c r="C561" s="125" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D561" s="125" t="str">
         <f>+VLOOKUP(C561,distribution!C$2:D$40,2,FALSE)</f>
         <v>Indicadores de Comercio interno en valores anuales, trimestrales y mensuales</v>
       </c>
       <c r="E561" s="125" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="F561" s="118" t="s">
         <v>10</v>
       </c>
       <c r="G561" s="118" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="H561" s="89" t="s">
         <v>401</v>
@@ -30290,7 +30290,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="73" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C80" s="161"/>
       <c r="D80" s="73" t="s">
@@ -30308,7 +30308,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="73" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C81" s="161"/>
       <c r="D81" s="73"/>
@@ -30320,7 +30320,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="73" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C82" s="161"/>
       <c r="D82" s="73"/>
@@ -30332,7 +30332,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="73" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="C83" s="161"/>
       <c r="D83" s="73"/>
@@ -30344,7 +30344,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="73" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="C84" s="161"/>
       <c r="D84" s="73"/>
@@ -30356,11 +30356,11 @@
         <v>84</v>
       </c>
       <c r="B85" s="73" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="C85" s="161"/>
       <c r="D85" s="73" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="E85" s="72">
         <v>1000</v>

</xml_diff>